<commit_message>
cap nhat nhanh main lan 3
</commit_message>
<xml_diff>
--- a/Masterwork_Task(Team01).xlsx
+++ b/Masterwork_Task(Team01).xlsx
@@ -479,17 +479,11 @@
     <xf borderId="10" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="6" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
     <xf borderId="8" fillId="5" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="8" fillId="6" fontId="6" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf borderId="10" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -503,11 +497,17 @@
     <xf borderId="7" fillId="5" fontId="7" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="8" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="8" fillId="6" fontId="7" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="8" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf borderId="8" fillId="6" fontId="6" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="8" fillId="6" fontId="6" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -994,7 +994,7 @@
         <v>45029.0</v>
       </c>
       <c r="E9" s="11">
-        <v>0.8</v>
+        <v>1.0</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>11</v>
@@ -1018,13 +1018,13 @@
       <c r="D10" s="10">
         <v>45029.0</v>
       </c>
-      <c r="E10" s="27">
-        <v>0.8</v>
+      <c r="E10" s="11">
+        <v>1.0</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="28"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="21"/>
       <c r="I10" s="22"/>
       <c r="J10" s="23"/>
@@ -1043,17 +1043,17 @@
       <c r="D11" s="10">
         <v>45029.0</v>
       </c>
-      <c r="E11" s="27">
-        <v>0.8</v>
+      <c r="E11" s="11">
+        <v>1.0</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="28"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="21"/>
       <c r="I11" s="22"/>
       <c r="J11" s="23"/>
-      <c r="K11" s="29" t="s">
+      <c r="K11" s="28" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1070,7 +1070,9 @@
       <c r="D12" s="10">
         <v>45031.0</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="11">
+        <v>1.0</v>
+      </c>
       <c r="F12" s="12" t="s">
         <v>11</v>
       </c>
@@ -1078,7 +1080,7 @@
       <c r="H12" s="21"/>
       <c r="I12" s="22"/>
       <c r="J12" s="23"/>
-      <c r="K12" s="29" t="s">
+      <c r="K12" s="28" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1086,7 +1088,7 @@
       <c r="A13" s="8">
         <v>12.0</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="29" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="10">
@@ -1095,7 +1097,9 @@
       <c r="D13" s="10">
         <v>45032.0</v>
       </c>
-      <c r="E13" s="30"/>
+      <c r="E13" s="11">
+        <v>1.0</v>
+      </c>
       <c r="F13" s="12" t="s">
         <v>11</v>
       </c>
@@ -1103,7 +1107,7 @@
       <c r="H13" s="21"/>
       <c r="I13" s="22"/>
       <c r="J13" s="23"/>
-      <c r="K13" s="29" t="s">
+      <c r="K13" s="28" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1111,7 +1115,7 @@
       <c r="A14" s="8">
         <v>13.0</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="29" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="10">
@@ -1120,7 +1124,9 @@
       <c r="D14" s="10">
         <v>45033.0</v>
       </c>
-      <c r="E14" s="30"/>
+      <c r="E14" s="11">
+        <v>1.0</v>
+      </c>
       <c r="F14" s="12" t="s">
         <v>11</v>
       </c>
@@ -1143,7 +1149,9 @@
       <c r="D15" s="10">
         <v>45034.0</v>
       </c>
-      <c r="E15" s="30"/>
+      <c r="E15" s="11">
+        <v>1.0</v>
+      </c>
       <c r="F15" s="12" t="s">
         <v>11</v>
       </c>
@@ -1151,7 +1159,7 @@
       <c r="H15" s="21"/>
       <c r="I15" s="22"/>
       <c r="J15" s="23"/>
-      <c r="K15" s="29" t="s">
+      <c r="K15" s="28" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1159,7 +1167,7 @@
       <c r="A16" s="8">
         <v>15.0</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="29" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="10">
@@ -1168,7 +1176,9 @@
       <c r="D16" s="10">
         <v>45035.0</v>
       </c>
-      <c r="E16" s="30"/>
+      <c r="E16" s="11">
+        <v>1.0</v>
+      </c>
       <c r="F16" s="12" t="s">
         <v>11</v>
       </c>
@@ -1176,75 +1186,81 @@
       <c r="H16" s="21"/>
       <c r="I16" s="22"/>
       <c r="J16" s="23"/>
-      <c r="K16" s="29" t="s">
+      <c r="K16" s="28" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" ht="15.0" customHeight="1">
-      <c r="A17" s="32">
+      <c r="A17" s="30">
         <v>16.0</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="32">
         <v>45028.0</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17" s="32">
         <v>45029.0</v>
       </c>
-      <c r="E17" s="35"/>
-      <c r="F17" s="36" t="s">
+      <c r="E17" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="F17" s="33" t="s">
         <v>33</v>
       </c>
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
       <c r="I17" s="22"/>
       <c r="J17" s="23"/>
-      <c r="K17" s="29" t="s">
+      <c r="K17" s="28" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" ht="15.0" customHeight="1">
-      <c r="A18" s="32">
+      <c r="A18" s="30">
         <v>17.0</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="32">
         <v>45030.0</v>
       </c>
-      <c r="D18" s="34">
+      <c r="D18" s="32">
         <v>45031.0</v>
       </c>
-      <c r="E18" s="35"/>
-      <c r="F18" s="36" t="s">
+      <c r="E18" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="F18" s="33" t="s">
         <v>33</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
       <c r="I18" s="22"/>
       <c r="J18" s="23"/>
-      <c r="K18" s="29" t="s">
+      <c r="K18" s="28" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" ht="15.0" customHeight="1">
-      <c r="A19" s="32">
+      <c r="A19" s="30">
         <v>18.0</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="34">
+      <c r="C19" s="32">
         <v>45032.0</v>
       </c>
-      <c r="D19" s="34">
+      <c r="D19" s="32">
         <v>45033.0</v>
       </c>
-      <c r="E19" s="35"/>
-      <c r="F19" s="36" t="s">
+      <c r="E19" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="F19" s="33" t="s">
         <v>33</v>
       </c>
       <c r="G19" s="21"/>
@@ -1254,20 +1270,20 @@
       <c r="K19" s="24"/>
     </row>
     <row r="20" ht="15.0" customHeight="1">
-      <c r="A20" s="32">
+      <c r="A20" s="30">
         <v>19.0</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="34">
+      <c r="C20" s="32">
         <v>45034.0</v>
       </c>
-      <c r="D20" s="34">
+      <c r="D20" s="32">
         <v>45035.0</v>
       </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36" t="s">
+      <c r="E20" s="34"/>
+      <c r="F20" s="33" t="s">
         <v>33</v>
       </c>
       <c r="G20" s="21"/>
@@ -1277,20 +1293,20 @@
       <c r="K20" s="24"/>
     </row>
     <row r="21" ht="15.0" customHeight="1">
-      <c r="A21" s="32">
+      <c r="A21" s="30">
         <v>20.0</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="34">
+      <c r="C21" s="32">
         <v>45036.0</v>
       </c>
-      <c r="D21" s="34">
+      <c r="D21" s="32">
         <v>45037.0</v>
       </c>
-      <c r="E21" s="35"/>
-      <c r="F21" s="36" t="s">
+      <c r="E21" s="34"/>
+      <c r="F21" s="33" t="s">
         <v>33</v>
       </c>
       <c r="G21" s="21"/>
@@ -1303,7 +1319,7 @@
       <c r="A22" s="8">
         <v>21.0</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="29" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="10">
@@ -1312,7 +1328,9 @@
       <c r="D22" s="10">
         <v>45039.0</v>
       </c>
-      <c r="E22" s="30"/>
+      <c r="E22" s="35">
+        <v>0.4</v>
+      </c>
       <c r="F22" s="12" t="s">
         <v>13</v>
       </c>
@@ -1326,7 +1344,7 @@
       <c r="A23" s="8">
         <v>22.0</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="29" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="10">
@@ -1335,7 +1353,7 @@
       <c r="D23" s="10">
         <v>45042.0</v>
       </c>
-      <c r="E23" s="30"/>
+      <c r="E23" s="36"/>
       <c r="F23" s="12" t="s">
         <v>13</v>
       </c>
@@ -1349,7 +1367,7 @@
       <c r="A24" s="8">
         <v>23.0</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="29" t="s">
         <v>42</v>
       </c>
       <c r="C24" s="10">
@@ -1358,7 +1376,7 @@
       <c r="D24" s="10">
         <v>45043.0</v>
       </c>
-      <c r="E24" s="30"/>
+      <c r="E24" s="36"/>
       <c r="F24" s="12" t="s">
         <v>13</v>
       </c>
@@ -4285,7 +4303,7 @@
       <c r="K996" s="37"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E10:E24">
+  <conditionalFormatting sqref="E20:E24">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>

</xml_diff>

<commit_message>
cap nhat file Task work
</commit_message>
<xml_diff>
--- a/Masterwork_Task(Team01).xlsx
+++ b/Masterwork_Task(Team01).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>No.</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>Our Clients</t>
+  </si>
+  <si>
+    <t>Minh + Quang</t>
+  </si>
+  <si>
+    <t>Using owl carousel</t>
   </si>
   <si>
     <t>Community</t>
@@ -161,7 +167,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd"/>
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mm"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -210,12 +216,6 @@
       <i/>
       <sz val="9.0"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9.0"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -401,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -488,20 +488,17 @@
     <xf borderId="10" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="5" fontId="7" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="7" fillId="5" fontId="6" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="8" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="6" fontId="7" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf borderId="8" fillId="6" fontId="6" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0"/>
@@ -509,7 +506,7 @@
     <xf borderId="8" fillId="6" fontId="6" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1261,20 +1258,22 @@
         <v>1.0</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
       <c r="I19" s="22"/>
       <c r="J19" s="23"/>
-      <c r="K19" s="24"/>
+      <c r="K19" s="28" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="20" ht="15.0" customHeight="1">
       <c r="A20" s="30">
         <v>19.0</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C20" s="32">
         <v>45034.0</v>
@@ -1282,7 +1281,9 @@
       <c r="D20" s="32">
         <v>45035.0</v>
       </c>
-      <c r="E20" s="34"/>
+      <c r="E20" s="11">
+        <v>1.0</v>
+      </c>
       <c r="F20" s="33" t="s">
         <v>33</v>
       </c>
@@ -1297,7 +1298,7 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C21" s="32">
         <v>45036.0</v>
@@ -1305,7 +1306,9 @@
       <c r="D21" s="32">
         <v>45037.0</v>
       </c>
-      <c r="E21" s="34"/>
+      <c r="E21" s="11">
+        <v>1.0</v>
+      </c>
       <c r="F21" s="33" t="s">
         <v>33</v>
       </c>
@@ -1320,7 +1323,7 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C22" s="10">
         <v>45038.0</v>
@@ -1328,11 +1331,11 @@
       <c r="D22" s="10">
         <v>45039.0</v>
       </c>
-      <c r="E22" s="35">
-        <v>0.4</v>
+      <c r="E22" s="11">
+        <v>1.0</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G22" s="21"/>
       <c r="H22" s="21"/>
@@ -1345,7 +1348,7 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C23" s="10">
         <v>45040.0</v>
@@ -1353,9 +1356,11 @@
       <c r="D23" s="10">
         <v>45042.0</v>
       </c>
-      <c r="E23" s="36"/>
+      <c r="E23" s="34">
+        <v>0.5</v>
+      </c>
       <c r="F23" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G23" s="21"/>
       <c r="H23" s="21"/>
@@ -1368,7 +1373,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C24" s="10">
         <v>45042.0</v>
@@ -1376,9 +1381,9 @@
       <c r="D24" s="10">
         <v>45043.0</v>
       </c>
-      <c r="E24" s="36"/>
+      <c r="E24" s="35"/>
       <c r="F24" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G24" s="21"/>
       <c r="H24" s="21"/>
@@ -1387,2923 +1392,2923 @@
       <c r="K24" s="24"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="K25" s="37"/>
+      <c r="K25" s="36"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="K26" s="37"/>
+      <c r="K26" s="36"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="K27" s="37"/>
+      <c r="K27" s="36"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="K28" s="37"/>
+      <c r="K28" s="36"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="K29" s="37"/>
+      <c r="K29" s="36"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="K30" s="37"/>
+      <c r="K30" s="36"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="K31" s="37"/>
+      <c r="K31" s="36"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="K32" s="37"/>
+      <c r="K32" s="36"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="K33" s="37"/>
+      <c r="K33" s="36"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="K34" s="37"/>
+      <c r="K34" s="36"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="K35" s="37"/>
+      <c r="K35" s="36"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="K36" s="37"/>
+      <c r="K36" s="36"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="K37" s="37"/>
+      <c r="K37" s="36"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="K38" s="37"/>
+      <c r="K38" s="36"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="K39" s="37"/>
+      <c r="K39" s="36"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="K40" s="37"/>
+      <c r="K40" s="36"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="K41" s="37"/>
+      <c r="K41" s="36"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="K42" s="37"/>
+      <c r="K42" s="36"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="K43" s="37"/>
+      <c r="K43" s="36"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="K44" s="37"/>
+      <c r="K44" s="36"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="K45" s="37"/>
+      <c r="K45" s="36"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
-      <c r="K46" s="37"/>
+      <c r="K46" s="36"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
-      <c r="K47" s="37"/>
+      <c r="K47" s="36"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="K48" s="37"/>
+      <c r="K48" s="36"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="K49" s="37"/>
+      <c r="K49" s="36"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
-      <c r="K50" s="37"/>
+      <c r="K50" s="36"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
-      <c r="K51" s="37"/>
+      <c r="K51" s="36"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
-      <c r="K52" s="37"/>
+      <c r="K52" s="36"/>
     </row>
     <row r="53" ht="14.25" customHeight="1">
-      <c r="K53" s="37"/>
+      <c r="K53" s="36"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
-      <c r="K54" s="37"/>
+      <c r="K54" s="36"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="K55" s="37"/>
+      <c r="K55" s="36"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
-      <c r="K56" s="37"/>
+      <c r="K56" s="36"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="K57" s="37"/>
+      <c r="K57" s="36"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="K58" s="37"/>
+      <c r="K58" s="36"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="K59" s="37"/>
+      <c r="K59" s="36"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="K60" s="37"/>
+      <c r="K60" s="36"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
-      <c r="K61" s="37"/>
+      <c r="K61" s="36"/>
     </row>
     <row r="62" ht="14.25" customHeight="1">
-      <c r="K62" s="37"/>
+      <c r="K62" s="36"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
-      <c r="K63" s="37"/>
+      <c r="K63" s="36"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
-      <c r="K64" s="37"/>
+      <c r="K64" s="36"/>
     </row>
     <row r="65" ht="14.25" customHeight="1">
-      <c r="K65" s="37"/>
+      <c r="K65" s="36"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
-      <c r="K66" s="37"/>
+      <c r="K66" s="36"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
-      <c r="K67" s="37"/>
+      <c r="K67" s="36"/>
     </row>
     <row r="68" ht="14.25" customHeight="1">
-      <c r="K68" s="37"/>
+      <c r="K68" s="36"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
-      <c r="K69" s="37"/>
+      <c r="K69" s="36"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
-      <c r="K70" s="37"/>
+      <c r="K70" s="36"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
-      <c r="K71" s="37"/>
+      <c r="K71" s="36"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
-      <c r="K72" s="37"/>
+      <c r="K72" s="36"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
-      <c r="K73" s="37"/>
+      <c r="K73" s="36"/>
     </row>
     <row r="74" ht="14.25" customHeight="1">
-      <c r="K74" s="37"/>
+      <c r="K74" s="36"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
-      <c r="K75" s="37"/>
+      <c r="K75" s="36"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
-      <c r="K76" s="37"/>
+      <c r="K76" s="36"/>
     </row>
     <row r="77" ht="14.25" customHeight="1">
-      <c r="K77" s="37"/>
+      <c r="K77" s="36"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
-      <c r="K78" s="37"/>
+      <c r="K78" s="36"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
-      <c r="K79" s="37"/>
+      <c r="K79" s="36"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
-      <c r="K80" s="37"/>
+      <c r="K80" s="36"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
-      <c r="K81" s="37"/>
+      <c r="K81" s="36"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
-      <c r="K82" s="37"/>
+      <c r="K82" s="36"/>
     </row>
     <row r="83" ht="14.25" customHeight="1">
-      <c r="K83" s="37"/>
+      <c r="K83" s="36"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
-      <c r="K84" s="37"/>
+      <c r="K84" s="36"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
-      <c r="K85" s="37"/>
+      <c r="K85" s="36"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
-      <c r="K86" s="37"/>
+      <c r="K86" s="36"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
-      <c r="K87" s="37"/>
+      <c r="K87" s="36"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
-      <c r="K88" s="37"/>
+      <c r="K88" s="36"/>
     </row>
     <row r="89" ht="14.25" customHeight="1">
-      <c r="K89" s="37"/>
+      <c r="K89" s="36"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
-      <c r="K90" s="37"/>
+      <c r="K90" s="36"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
-      <c r="K91" s="37"/>
+      <c r="K91" s="36"/>
     </row>
     <row r="92" ht="14.25" customHeight="1">
-      <c r="K92" s="37"/>
+      <c r="K92" s="36"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
-      <c r="K93" s="37"/>
+      <c r="K93" s="36"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
-      <c r="K94" s="37"/>
+      <c r="K94" s="36"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="K95" s="37"/>
+      <c r="K95" s="36"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
-      <c r="K96" s="37"/>
+      <c r="K96" s="36"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
-      <c r="K97" s="37"/>
+      <c r="K97" s="36"/>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="K98" s="37"/>
+      <c r="K98" s="36"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
-      <c r="K99" s="37"/>
+      <c r="K99" s="36"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
-      <c r="K100" s="37"/>
+      <c r="K100" s="36"/>
     </row>
     <row r="101" ht="14.25" customHeight="1">
-      <c r="K101" s="37"/>
+      <c r="K101" s="36"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
-      <c r="K102" s="37"/>
+      <c r="K102" s="36"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
-      <c r="K103" s="37"/>
+      <c r="K103" s="36"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
-      <c r="K104" s="37"/>
+      <c r="K104" s="36"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
-      <c r="K105" s="37"/>
+      <c r="K105" s="36"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
-      <c r="K106" s="37"/>
+      <c r="K106" s="36"/>
     </row>
     <row r="107" ht="14.25" customHeight="1">
-      <c r="K107" s="37"/>
+      <c r="K107" s="36"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
-      <c r="K108" s="37"/>
+      <c r="K108" s="36"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
-      <c r="K109" s="37"/>
+      <c r="K109" s="36"/>
     </row>
     <row r="110" ht="14.25" customHeight="1">
-      <c r="K110" s="37"/>
+      <c r="K110" s="36"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
-      <c r="K111" s="37"/>
+      <c r="K111" s="36"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
-      <c r="K112" s="37"/>
+      <c r="K112" s="36"/>
     </row>
     <row r="113" ht="14.25" customHeight="1">
-      <c r="K113" s="37"/>
+      <c r="K113" s="36"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
-      <c r="K114" s="37"/>
+      <c r="K114" s="36"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
-      <c r="K115" s="37"/>
+      <c r="K115" s="36"/>
     </row>
     <row r="116" ht="14.25" customHeight="1">
-      <c r="K116" s="37"/>
+      <c r="K116" s="36"/>
     </row>
     <row r="117" ht="14.25" customHeight="1">
-      <c r="K117" s="37"/>
+      <c r="K117" s="36"/>
     </row>
     <row r="118" ht="14.25" customHeight="1">
-      <c r="K118" s="37"/>
+      <c r="K118" s="36"/>
     </row>
     <row r="119" ht="14.25" customHeight="1">
-      <c r="K119" s="37"/>
+      <c r="K119" s="36"/>
     </row>
     <row r="120" ht="14.25" customHeight="1">
-      <c r="K120" s="37"/>
+      <c r="K120" s="36"/>
     </row>
     <row r="121" ht="14.25" customHeight="1">
-      <c r="K121" s="37"/>
+      <c r="K121" s="36"/>
     </row>
     <row r="122" ht="14.25" customHeight="1">
-      <c r="K122" s="37"/>
+      <c r="K122" s="36"/>
     </row>
     <row r="123" ht="14.25" customHeight="1">
-      <c r="K123" s="37"/>
+      <c r="K123" s="36"/>
     </row>
     <row r="124" ht="14.25" customHeight="1">
-      <c r="K124" s="37"/>
+      <c r="K124" s="36"/>
     </row>
     <row r="125" ht="14.25" customHeight="1">
-      <c r="K125" s="37"/>
+      <c r="K125" s="36"/>
     </row>
     <row r="126" ht="14.25" customHeight="1">
-      <c r="K126" s="37"/>
+      <c r="K126" s="36"/>
     </row>
     <row r="127" ht="14.25" customHeight="1">
-      <c r="K127" s="37"/>
+      <c r="K127" s="36"/>
     </row>
     <row r="128" ht="14.25" customHeight="1">
-      <c r="K128" s="37"/>
+      <c r="K128" s="36"/>
     </row>
     <row r="129" ht="14.25" customHeight="1">
-      <c r="K129" s="37"/>
+      <c r="K129" s="36"/>
     </row>
     <row r="130" ht="14.25" customHeight="1">
-      <c r="K130" s="37"/>
+      <c r="K130" s="36"/>
     </row>
     <row r="131" ht="14.25" customHeight="1">
-      <c r="K131" s="37"/>
+      <c r="K131" s="36"/>
     </row>
     <row r="132" ht="14.25" customHeight="1">
-      <c r="K132" s="37"/>
+      <c r="K132" s="36"/>
     </row>
     <row r="133" ht="14.25" customHeight="1">
-      <c r="K133" s="37"/>
+      <c r="K133" s="36"/>
     </row>
     <row r="134" ht="14.25" customHeight="1">
-      <c r="K134" s="37"/>
+      <c r="K134" s="36"/>
     </row>
     <row r="135" ht="14.25" customHeight="1">
-      <c r="K135" s="37"/>
+      <c r="K135" s="36"/>
     </row>
     <row r="136" ht="14.25" customHeight="1">
-      <c r="K136" s="37"/>
+      <c r="K136" s="36"/>
     </row>
     <row r="137" ht="14.25" customHeight="1">
-      <c r="K137" s="37"/>
+      <c r="K137" s="36"/>
     </row>
     <row r="138" ht="14.25" customHeight="1">
-      <c r="K138" s="37"/>
+      <c r="K138" s="36"/>
     </row>
     <row r="139" ht="14.25" customHeight="1">
-      <c r="K139" s="37"/>
+      <c r="K139" s="36"/>
     </row>
     <row r="140" ht="14.25" customHeight="1">
-      <c r="K140" s="37"/>
+      <c r="K140" s="36"/>
     </row>
     <row r="141" ht="14.25" customHeight="1">
-      <c r="K141" s="37"/>
+      <c r="K141" s="36"/>
     </row>
     <row r="142" ht="14.25" customHeight="1">
-      <c r="K142" s="37"/>
+      <c r="K142" s="36"/>
     </row>
     <row r="143" ht="14.25" customHeight="1">
-      <c r="K143" s="37"/>
+      <c r="K143" s="36"/>
     </row>
     <row r="144" ht="14.25" customHeight="1">
-      <c r="K144" s="37"/>
+      <c r="K144" s="36"/>
     </row>
     <row r="145" ht="14.25" customHeight="1">
-      <c r="K145" s="37"/>
+      <c r="K145" s="36"/>
     </row>
     <row r="146" ht="14.25" customHeight="1">
-      <c r="K146" s="37"/>
+      <c r="K146" s="36"/>
     </row>
     <row r="147" ht="14.25" customHeight="1">
-      <c r="K147" s="37"/>
+      <c r="K147" s="36"/>
     </row>
     <row r="148" ht="14.25" customHeight="1">
-      <c r="K148" s="37"/>
+      <c r="K148" s="36"/>
     </row>
     <row r="149" ht="14.25" customHeight="1">
-      <c r="K149" s="37"/>
+      <c r="K149" s="36"/>
     </row>
     <row r="150" ht="14.25" customHeight="1">
-      <c r="K150" s="37"/>
+      <c r="K150" s="36"/>
     </row>
     <row r="151" ht="14.25" customHeight="1">
-      <c r="K151" s="37"/>
+      <c r="K151" s="36"/>
     </row>
     <row r="152" ht="14.25" customHeight="1">
-      <c r="K152" s="37"/>
+      <c r="K152" s="36"/>
     </row>
     <row r="153" ht="14.25" customHeight="1">
-      <c r="K153" s="37"/>
+      <c r="K153" s="36"/>
     </row>
     <row r="154" ht="14.25" customHeight="1">
-      <c r="K154" s="37"/>
+      <c r="K154" s="36"/>
     </row>
     <row r="155" ht="14.25" customHeight="1">
-      <c r="K155" s="37"/>
+      <c r="K155" s="36"/>
     </row>
     <row r="156" ht="14.25" customHeight="1">
-      <c r="K156" s="37"/>
+      <c r="K156" s="36"/>
     </row>
     <row r="157" ht="14.25" customHeight="1">
-      <c r="K157" s="37"/>
+      <c r="K157" s="36"/>
     </row>
     <row r="158" ht="14.25" customHeight="1">
-      <c r="K158" s="37"/>
+      <c r="K158" s="36"/>
     </row>
     <row r="159" ht="14.25" customHeight="1">
-      <c r="K159" s="37"/>
+      <c r="K159" s="36"/>
     </row>
     <row r="160" ht="14.25" customHeight="1">
-      <c r="K160" s="37"/>
+      <c r="K160" s="36"/>
     </row>
     <row r="161" ht="14.25" customHeight="1">
-      <c r="K161" s="37"/>
+      <c r="K161" s="36"/>
     </row>
     <row r="162" ht="14.25" customHeight="1">
-      <c r="K162" s="37"/>
+      <c r="K162" s="36"/>
     </row>
     <row r="163" ht="14.25" customHeight="1">
-      <c r="K163" s="37"/>
+      <c r="K163" s="36"/>
     </row>
     <row r="164" ht="14.25" customHeight="1">
-      <c r="K164" s="37"/>
+      <c r="K164" s="36"/>
     </row>
     <row r="165" ht="14.25" customHeight="1">
-      <c r="K165" s="37"/>
+      <c r="K165" s="36"/>
     </row>
     <row r="166" ht="14.25" customHeight="1">
-      <c r="K166" s="37"/>
+      <c r="K166" s="36"/>
     </row>
     <row r="167" ht="14.25" customHeight="1">
-      <c r="K167" s="37"/>
+      <c r="K167" s="36"/>
     </row>
     <row r="168" ht="14.25" customHeight="1">
-      <c r="K168" s="37"/>
+      <c r="K168" s="36"/>
     </row>
     <row r="169" ht="14.25" customHeight="1">
-      <c r="K169" s="37"/>
+      <c r="K169" s="36"/>
     </row>
     <row r="170" ht="14.25" customHeight="1">
-      <c r="K170" s="37"/>
+      <c r="K170" s="36"/>
     </row>
     <row r="171" ht="14.25" customHeight="1">
-      <c r="K171" s="37"/>
+      <c r="K171" s="36"/>
     </row>
     <row r="172" ht="14.25" customHeight="1">
-      <c r="K172" s="37"/>
+      <c r="K172" s="36"/>
     </row>
     <row r="173" ht="14.25" customHeight="1">
-      <c r="K173" s="37"/>
+      <c r="K173" s="36"/>
     </row>
     <row r="174" ht="14.25" customHeight="1">
-      <c r="K174" s="37"/>
+      <c r="K174" s="36"/>
     </row>
     <row r="175" ht="14.25" customHeight="1">
-      <c r="K175" s="37"/>
+      <c r="K175" s="36"/>
     </row>
     <row r="176" ht="14.25" customHeight="1">
-      <c r="K176" s="37"/>
+      <c r="K176" s="36"/>
     </row>
     <row r="177" ht="14.25" customHeight="1">
-      <c r="K177" s="37"/>
+      <c r="K177" s="36"/>
     </row>
     <row r="178" ht="14.25" customHeight="1">
-      <c r="K178" s="37"/>
+      <c r="K178" s="36"/>
     </row>
     <row r="179" ht="14.25" customHeight="1">
-      <c r="K179" s="37"/>
+      <c r="K179" s="36"/>
     </row>
     <row r="180" ht="14.25" customHeight="1">
-      <c r="K180" s="37"/>
+      <c r="K180" s="36"/>
     </row>
     <row r="181" ht="14.25" customHeight="1">
-      <c r="K181" s="37"/>
+      <c r="K181" s="36"/>
     </row>
     <row r="182" ht="14.25" customHeight="1">
-      <c r="K182" s="37"/>
+      <c r="K182" s="36"/>
     </row>
     <row r="183" ht="14.25" customHeight="1">
-      <c r="K183" s="37"/>
+      <c r="K183" s="36"/>
     </row>
     <row r="184" ht="14.25" customHeight="1">
-      <c r="K184" s="37"/>
+      <c r="K184" s="36"/>
     </row>
     <row r="185" ht="14.25" customHeight="1">
-      <c r="K185" s="37"/>
+      <c r="K185" s="36"/>
     </row>
     <row r="186" ht="14.25" customHeight="1">
-      <c r="K186" s="37"/>
+      <c r="K186" s="36"/>
     </row>
     <row r="187" ht="14.25" customHeight="1">
-      <c r="K187" s="37"/>
+      <c r="K187" s="36"/>
     </row>
     <row r="188" ht="14.25" customHeight="1">
-      <c r="K188" s="37"/>
+      <c r="K188" s="36"/>
     </row>
     <row r="189" ht="14.25" customHeight="1">
-      <c r="K189" s="37"/>
+      <c r="K189" s="36"/>
     </row>
     <row r="190" ht="14.25" customHeight="1">
-      <c r="K190" s="37"/>
+      <c r="K190" s="36"/>
     </row>
     <row r="191" ht="14.25" customHeight="1">
-      <c r="K191" s="37"/>
+      <c r="K191" s="36"/>
     </row>
     <row r="192" ht="14.25" customHeight="1">
-      <c r="K192" s="37"/>
+      <c r="K192" s="36"/>
     </row>
     <row r="193" ht="14.25" customHeight="1">
-      <c r="K193" s="37"/>
+      <c r="K193" s="36"/>
     </row>
     <row r="194" ht="14.25" customHeight="1">
-      <c r="K194" s="37"/>
+      <c r="K194" s="36"/>
     </row>
     <row r="195" ht="14.25" customHeight="1">
-      <c r="K195" s="37"/>
+      <c r="K195" s="36"/>
     </row>
     <row r="196" ht="14.25" customHeight="1">
-      <c r="K196" s="37"/>
+      <c r="K196" s="36"/>
     </row>
     <row r="197" ht="14.25" customHeight="1">
-      <c r="K197" s="37"/>
+      <c r="K197" s="36"/>
     </row>
     <row r="198" ht="14.25" customHeight="1">
-      <c r="K198" s="37"/>
+      <c r="K198" s="36"/>
     </row>
     <row r="199" ht="14.25" customHeight="1">
-      <c r="K199" s="37"/>
+      <c r="K199" s="36"/>
     </row>
     <row r="200" ht="14.25" customHeight="1">
-      <c r="K200" s="37"/>
+      <c r="K200" s="36"/>
     </row>
     <row r="201" ht="14.25" customHeight="1">
-      <c r="K201" s="37"/>
+      <c r="K201" s="36"/>
     </row>
     <row r="202" ht="14.25" customHeight="1">
-      <c r="K202" s="37"/>
+      <c r="K202" s="36"/>
     </row>
     <row r="203" ht="14.25" customHeight="1">
-      <c r="K203" s="37"/>
+      <c r="K203" s="36"/>
     </row>
     <row r="204" ht="14.25" customHeight="1">
-      <c r="K204" s="37"/>
+      <c r="K204" s="36"/>
     </row>
     <row r="205" ht="14.25" customHeight="1">
-      <c r="K205" s="37"/>
+      <c r="K205" s="36"/>
     </row>
     <row r="206" ht="14.25" customHeight="1">
-      <c r="K206" s="37"/>
+      <c r="K206" s="36"/>
     </row>
     <row r="207" ht="14.25" customHeight="1">
-      <c r="K207" s="37"/>
+      <c r="K207" s="36"/>
     </row>
     <row r="208" ht="14.25" customHeight="1">
-      <c r="K208" s="37"/>
+      <c r="K208" s="36"/>
     </row>
     <row r="209" ht="14.25" customHeight="1">
-      <c r="K209" s="37"/>
+      <c r="K209" s="36"/>
     </row>
     <row r="210" ht="14.25" customHeight="1">
-      <c r="K210" s="37"/>
+      <c r="K210" s="36"/>
     </row>
     <row r="211" ht="14.25" customHeight="1">
-      <c r="K211" s="37"/>
+      <c r="K211" s="36"/>
     </row>
     <row r="212" ht="14.25" customHeight="1">
-      <c r="K212" s="37"/>
+      <c r="K212" s="36"/>
     </row>
     <row r="213" ht="14.25" customHeight="1">
-      <c r="K213" s="37"/>
+      <c r="K213" s="36"/>
     </row>
     <row r="214" ht="14.25" customHeight="1">
-      <c r="K214" s="37"/>
+      <c r="K214" s="36"/>
     </row>
     <row r="215" ht="14.25" customHeight="1">
-      <c r="K215" s="37"/>
+      <c r="K215" s="36"/>
     </row>
     <row r="216" ht="14.25" customHeight="1">
-      <c r="K216" s="37"/>
+      <c r="K216" s="36"/>
     </row>
     <row r="217" ht="14.25" customHeight="1">
-      <c r="K217" s="37"/>
+      <c r="K217" s="36"/>
     </row>
     <row r="218" ht="14.25" customHeight="1">
-      <c r="K218" s="37"/>
+      <c r="K218" s="36"/>
     </row>
     <row r="219" ht="14.25" customHeight="1">
-      <c r="K219" s="37"/>
+      <c r="K219" s="36"/>
     </row>
     <row r="220" ht="14.25" customHeight="1">
-      <c r="K220" s="37"/>
+      <c r="K220" s="36"/>
     </row>
     <row r="221" ht="14.25" customHeight="1">
-      <c r="K221" s="37"/>
+      <c r="K221" s="36"/>
     </row>
     <row r="222" ht="14.25" customHeight="1">
-      <c r="K222" s="37"/>
+      <c r="K222" s="36"/>
     </row>
     <row r="223" ht="14.25" customHeight="1">
-      <c r="K223" s="37"/>
+      <c r="K223" s="36"/>
     </row>
     <row r="224" ht="14.25" customHeight="1">
-      <c r="K224" s="37"/>
+      <c r="K224" s="36"/>
     </row>
     <row r="225" ht="14.25" customHeight="1">
-      <c r="K225" s="37"/>
+      <c r="K225" s="36"/>
     </row>
     <row r="226" ht="14.25" customHeight="1">
-      <c r="K226" s="37"/>
+      <c r="K226" s="36"/>
     </row>
     <row r="227" ht="14.25" customHeight="1">
-      <c r="K227" s="37"/>
+      <c r="K227" s="36"/>
     </row>
     <row r="228" ht="14.25" customHeight="1">
-      <c r="K228" s="37"/>
+      <c r="K228" s="36"/>
     </row>
     <row r="229" ht="14.25" customHeight="1">
-      <c r="K229" s="37"/>
+      <c r="K229" s="36"/>
     </row>
     <row r="230" ht="14.25" customHeight="1">
-      <c r="K230" s="37"/>
+      <c r="K230" s="36"/>
     </row>
     <row r="231" ht="14.25" customHeight="1">
-      <c r="K231" s="37"/>
+      <c r="K231" s="36"/>
     </row>
     <row r="232" ht="14.25" customHeight="1">
-      <c r="K232" s="37"/>
+      <c r="K232" s="36"/>
     </row>
     <row r="233" ht="14.25" customHeight="1">
-      <c r="K233" s="37"/>
+      <c r="K233" s="36"/>
     </row>
     <row r="234" ht="14.25" customHeight="1">
-      <c r="K234" s="37"/>
+      <c r="K234" s="36"/>
     </row>
     <row r="235" ht="14.25" customHeight="1">
-      <c r="K235" s="37"/>
+      <c r="K235" s="36"/>
     </row>
     <row r="236" ht="14.25" customHeight="1">
-      <c r="K236" s="37"/>
+      <c r="K236" s="36"/>
     </row>
     <row r="237" ht="14.25" customHeight="1">
-      <c r="K237" s="37"/>
+      <c r="K237" s="36"/>
     </row>
     <row r="238" ht="14.25" customHeight="1">
-      <c r="K238" s="37"/>
+      <c r="K238" s="36"/>
     </row>
     <row r="239" ht="14.25" customHeight="1">
-      <c r="K239" s="37"/>
+      <c r="K239" s="36"/>
     </row>
     <row r="240" ht="14.25" customHeight="1">
-      <c r="K240" s="37"/>
+      <c r="K240" s="36"/>
     </row>
     <row r="241" ht="14.25" customHeight="1">
-      <c r="K241" s="37"/>
+      <c r="K241" s="36"/>
     </row>
     <row r="242" ht="14.25" customHeight="1">
-      <c r="K242" s="37"/>
+      <c r="K242" s="36"/>
     </row>
     <row r="243" ht="14.25" customHeight="1">
-      <c r="K243" s="37"/>
+      <c r="K243" s="36"/>
     </row>
     <row r="244" ht="14.25" customHeight="1">
-      <c r="K244" s="37"/>
+      <c r="K244" s="36"/>
     </row>
     <row r="245" ht="14.25" customHeight="1">
-      <c r="K245" s="37"/>
+      <c r="K245" s="36"/>
     </row>
     <row r="246" ht="14.25" customHeight="1">
-      <c r="K246" s="37"/>
+      <c r="K246" s="36"/>
     </row>
     <row r="247" ht="14.25" customHeight="1">
-      <c r="K247" s="37"/>
+      <c r="K247" s="36"/>
     </row>
     <row r="248" ht="14.25" customHeight="1">
-      <c r="K248" s="37"/>
+      <c r="K248" s="36"/>
     </row>
     <row r="249" ht="14.25" customHeight="1">
-      <c r="K249" s="37"/>
+      <c r="K249" s="36"/>
     </row>
     <row r="250" ht="14.25" customHeight="1">
-      <c r="K250" s="37"/>
+      <c r="K250" s="36"/>
     </row>
     <row r="251" ht="14.25" customHeight="1">
-      <c r="K251" s="37"/>
+      <c r="K251" s="36"/>
     </row>
     <row r="252" ht="14.25" customHeight="1">
-      <c r="K252" s="37"/>
+      <c r="K252" s="36"/>
     </row>
     <row r="253" ht="14.25" customHeight="1">
-      <c r="K253" s="37"/>
+      <c r="K253" s="36"/>
     </row>
     <row r="254" ht="14.25" customHeight="1">
-      <c r="K254" s="37"/>
+      <c r="K254" s="36"/>
     </row>
     <row r="255" ht="14.25" customHeight="1">
-      <c r="K255" s="37"/>
+      <c r="K255" s="36"/>
     </row>
     <row r="256" ht="14.25" customHeight="1">
-      <c r="K256" s="37"/>
+      <c r="K256" s="36"/>
     </row>
     <row r="257" ht="14.25" customHeight="1">
-      <c r="K257" s="37"/>
+      <c r="K257" s="36"/>
     </row>
     <row r="258" ht="14.25" customHeight="1">
-      <c r="K258" s="37"/>
+      <c r="K258" s="36"/>
     </row>
     <row r="259" ht="14.25" customHeight="1">
-      <c r="K259" s="37"/>
+      <c r="K259" s="36"/>
     </row>
     <row r="260" ht="14.25" customHeight="1">
-      <c r="K260" s="37"/>
+      <c r="K260" s="36"/>
     </row>
     <row r="261" ht="14.25" customHeight="1">
-      <c r="K261" s="37"/>
+      <c r="K261" s="36"/>
     </row>
     <row r="262" ht="14.25" customHeight="1">
-      <c r="K262" s="37"/>
+      <c r="K262" s="36"/>
     </row>
     <row r="263" ht="14.25" customHeight="1">
-      <c r="K263" s="37"/>
+      <c r="K263" s="36"/>
     </row>
     <row r="264" ht="14.25" customHeight="1">
-      <c r="K264" s="37"/>
+      <c r="K264" s="36"/>
     </row>
     <row r="265" ht="14.25" customHeight="1">
-      <c r="K265" s="37"/>
+      <c r="K265" s="36"/>
     </row>
     <row r="266" ht="14.25" customHeight="1">
-      <c r="K266" s="37"/>
+      <c r="K266" s="36"/>
     </row>
     <row r="267" ht="14.25" customHeight="1">
-      <c r="K267" s="37"/>
+      <c r="K267" s="36"/>
     </row>
     <row r="268" ht="14.25" customHeight="1">
-      <c r="K268" s="37"/>
+      <c r="K268" s="36"/>
     </row>
     <row r="269" ht="14.25" customHeight="1">
-      <c r="K269" s="37"/>
+      <c r="K269" s="36"/>
     </row>
     <row r="270" ht="14.25" customHeight="1">
-      <c r="K270" s="37"/>
+      <c r="K270" s="36"/>
     </row>
     <row r="271" ht="14.25" customHeight="1">
-      <c r="K271" s="37"/>
+      <c r="K271" s="36"/>
     </row>
     <row r="272" ht="14.25" customHeight="1">
-      <c r="K272" s="37"/>
+      <c r="K272" s="36"/>
     </row>
     <row r="273" ht="14.25" customHeight="1">
-      <c r="K273" s="37"/>
+      <c r="K273" s="36"/>
     </row>
     <row r="274" ht="14.25" customHeight="1">
-      <c r="K274" s="37"/>
+      <c r="K274" s="36"/>
     </row>
     <row r="275" ht="14.25" customHeight="1">
-      <c r="K275" s="37"/>
+      <c r="K275" s="36"/>
     </row>
     <row r="276" ht="14.25" customHeight="1">
-      <c r="K276" s="37"/>
+      <c r="K276" s="36"/>
     </row>
     <row r="277" ht="14.25" customHeight="1">
-      <c r="K277" s="37"/>
+      <c r="K277" s="36"/>
     </row>
     <row r="278" ht="14.25" customHeight="1">
-      <c r="K278" s="37"/>
+      <c r="K278" s="36"/>
     </row>
     <row r="279" ht="14.25" customHeight="1">
-      <c r="K279" s="37"/>
+      <c r="K279" s="36"/>
     </row>
     <row r="280" ht="14.25" customHeight="1">
-      <c r="K280" s="37"/>
+      <c r="K280" s="36"/>
     </row>
     <row r="281" ht="14.25" customHeight="1">
-      <c r="K281" s="37"/>
+      <c r="K281" s="36"/>
     </row>
     <row r="282" ht="14.25" customHeight="1">
-      <c r="K282" s="37"/>
+      <c r="K282" s="36"/>
     </row>
     <row r="283" ht="14.25" customHeight="1">
-      <c r="K283" s="37"/>
+      <c r="K283" s="36"/>
     </row>
     <row r="284" ht="14.25" customHeight="1">
-      <c r="K284" s="37"/>
+      <c r="K284" s="36"/>
     </row>
     <row r="285" ht="14.25" customHeight="1">
-      <c r="K285" s="37"/>
+      <c r="K285" s="36"/>
     </row>
     <row r="286" ht="14.25" customHeight="1">
-      <c r="K286" s="37"/>
+      <c r="K286" s="36"/>
     </row>
     <row r="287" ht="14.25" customHeight="1">
-      <c r="K287" s="37"/>
+      <c r="K287" s="36"/>
     </row>
     <row r="288" ht="14.25" customHeight="1">
-      <c r="K288" s="37"/>
+      <c r="K288" s="36"/>
     </row>
     <row r="289" ht="14.25" customHeight="1">
-      <c r="K289" s="37"/>
+      <c r="K289" s="36"/>
     </row>
     <row r="290" ht="14.25" customHeight="1">
-      <c r="K290" s="37"/>
+      <c r="K290" s="36"/>
     </row>
     <row r="291" ht="14.25" customHeight="1">
-      <c r="K291" s="37"/>
+      <c r="K291" s="36"/>
     </row>
     <row r="292" ht="14.25" customHeight="1">
-      <c r="K292" s="37"/>
+      <c r="K292" s="36"/>
     </row>
     <row r="293" ht="14.25" customHeight="1">
-      <c r="K293" s="37"/>
+      <c r="K293" s="36"/>
     </row>
     <row r="294" ht="14.25" customHeight="1">
-      <c r="K294" s="37"/>
+      <c r="K294" s="36"/>
     </row>
     <row r="295" ht="14.25" customHeight="1">
-      <c r="K295" s="37"/>
+      <c r="K295" s="36"/>
     </row>
     <row r="296" ht="14.25" customHeight="1">
-      <c r="K296" s="37"/>
+      <c r="K296" s="36"/>
     </row>
     <row r="297" ht="14.25" customHeight="1">
-      <c r="K297" s="37"/>
+      <c r="K297" s="36"/>
     </row>
     <row r="298" ht="14.25" customHeight="1">
-      <c r="K298" s="37"/>
+      <c r="K298" s="36"/>
     </row>
     <row r="299" ht="14.25" customHeight="1">
-      <c r="K299" s="37"/>
+      <c r="K299" s="36"/>
     </row>
     <row r="300" ht="14.25" customHeight="1">
-      <c r="K300" s="37"/>
+      <c r="K300" s="36"/>
     </row>
     <row r="301" ht="14.25" customHeight="1">
-      <c r="K301" s="37"/>
+      <c r="K301" s="36"/>
     </row>
     <row r="302" ht="14.25" customHeight="1">
-      <c r="K302" s="37"/>
+      <c r="K302" s="36"/>
     </row>
     <row r="303" ht="14.25" customHeight="1">
-      <c r="K303" s="37"/>
+      <c r="K303" s="36"/>
     </row>
     <row r="304" ht="14.25" customHeight="1">
-      <c r="K304" s="37"/>
+      <c r="K304" s="36"/>
     </row>
     <row r="305" ht="14.25" customHeight="1">
-      <c r="K305" s="37"/>
+      <c r="K305" s="36"/>
     </row>
     <row r="306" ht="14.25" customHeight="1">
-      <c r="K306" s="37"/>
+      <c r="K306" s="36"/>
     </row>
     <row r="307" ht="14.25" customHeight="1">
-      <c r="K307" s="37"/>
+      <c r="K307" s="36"/>
     </row>
     <row r="308" ht="14.25" customHeight="1">
-      <c r="K308" s="37"/>
+      <c r="K308" s="36"/>
     </row>
     <row r="309" ht="14.25" customHeight="1">
-      <c r="K309" s="37"/>
+      <c r="K309" s="36"/>
     </row>
     <row r="310" ht="14.25" customHeight="1">
-      <c r="K310" s="37"/>
+      <c r="K310" s="36"/>
     </row>
     <row r="311" ht="14.25" customHeight="1">
-      <c r="K311" s="37"/>
+      <c r="K311" s="36"/>
     </row>
     <row r="312" ht="14.25" customHeight="1">
-      <c r="K312" s="37"/>
+      <c r="K312" s="36"/>
     </row>
     <row r="313" ht="14.25" customHeight="1">
-      <c r="K313" s="37"/>
+      <c r="K313" s="36"/>
     </row>
     <row r="314" ht="14.25" customHeight="1">
-      <c r="K314" s="37"/>
+      <c r="K314" s="36"/>
     </row>
     <row r="315" ht="14.25" customHeight="1">
-      <c r="K315" s="37"/>
+      <c r="K315" s="36"/>
     </row>
     <row r="316" ht="14.25" customHeight="1">
-      <c r="K316" s="37"/>
+      <c r="K316" s="36"/>
     </row>
     <row r="317" ht="14.25" customHeight="1">
-      <c r="K317" s="37"/>
+      <c r="K317" s="36"/>
     </row>
     <row r="318" ht="14.25" customHeight="1">
-      <c r="K318" s="37"/>
+      <c r="K318" s="36"/>
     </row>
     <row r="319" ht="14.25" customHeight="1">
-      <c r="K319" s="37"/>
+      <c r="K319" s="36"/>
     </row>
     <row r="320" ht="14.25" customHeight="1">
-      <c r="K320" s="37"/>
+      <c r="K320" s="36"/>
     </row>
     <row r="321" ht="14.25" customHeight="1">
-      <c r="K321" s="37"/>
+      <c r="K321" s="36"/>
     </row>
     <row r="322" ht="14.25" customHeight="1">
-      <c r="K322" s="37"/>
+      <c r="K322" s="36"/>
     </row>
     <row r="323" ht="14.25" customHeight="1">
-      <c r="K323" s="37"/>
+      <c r="K323" s="36"/>
     </row>
     <row r="324" ht="14.25" customHeight="1">
-      <c r="K324" s="37"/>
+      <c r="K324" s="36"/>
     </row>
     <row r="325" ht="14.25" customHeight="1">
-      <c r="K325" s="37"/>
+      <c r="K325" s="36"/>
     </row>
     <row r="326" ht="14.25" customHeight="1">
-      <c r="K326" s="37"/>
+      <c r="K326" s="36"/>
     </row>
     <row r="327" ht="14.25" customHeight="1">
-      <c r="K327" s="37"/>
+      <c r="K327" s="36"/>
     </row>
     <row r="328" ht="14.25" customHeight="1">
-      <c r="K328" s="37"/>
+      <c r="K328" s="36"/>
     </row>
     <row r="329" ht="14.25" customHeight="1">
-      <c r="K329" s="37"/>
+      <c r="K329" s="36"/>
     </row>
     <row r="330" ht="14.25" customHeight="1">
-      <c r="K330" s="37"/>
+      <c r="K330" s="36"/>
     </row>
     <row r="331" ht="14.25" customHeight="1">
-      <c r="K331" s="37"/>
+      <c r="K331" s="36"/>
     </row>
     <row r="332" ht="14.25" customHeight="1">
-      <c r="K332" s="37"/>
+      <c r="K332" s="36"/>
     </row>
     <row r="333" ht="14.25" customHeight="1">
-      <c r="K333" s="37"/>
+      <c r="K333" s="36"/>
     </row>
     <row r="334" ht="14.25" customHeight="1">
-      <c r="K334" s="37"/>
+      <c r="K334" s="36"/>
     </row>
     <row r="335" ht="14.25" customHeight="1">
-      <c r="K335" s="37"/>
+      <c r="K335" s="36"/>
     </row>
     <row r="336" ht="14.25" customHeight="1">
-      <c r="K336" s="37"/>
+      <c r="K336" s="36"/>
     </row>
     <row r="337" ht="14.25" customHeight="1">
-      <c r="K337" s="37"/>
+      <c r="K337" s="36"/>
     </row>
     <row r="338" ht="14.25" customHeight="1">
-      <c r="K338" s="37"/>
+      <c r="K338" s="36"/>
     </row>
     <row r="339" ht="14.25" customHeight="1">
-      <c r="K339" s="37"/>
+      <c r="K339" s="36"/>
     </row>
     <row r="340" ht="14.25" customHeight="1">
-      <c r="K340" s="37"/>
+      <c r="K340" s="36"/>
     </row>
     <row r="341" ht="14.25" customHeight="1">
-      <c r="K341" s="37"/>
+      <c r="K341" s="36"/>
     </row>
     <row r="342" ht="14.25" customHeight="1">
-      <c r="K342" s="37"/>
+      <c r="K342" s="36"/>
     </row>
     <row r="343" ht="14.25" customHeight="1">
-      <c r="K343" s="37"/>
+      <c r="K343" s="36"/>
     </row>
     <row r="344" ht="14.25" customHeight="1">
-      <c r="K344" s="37"/>
+      <c r="K344" s="36"/>
     </row>
     <row r="345" ht="14.25" customHeight="1">
-      <c r="K345" s="37"/>
+      <c r="K345" s="36"/>
     </row>
     <row r="346" ht="14.25" customHeight="1">
-      <c r="K346" s="37"/>
+      <c r="K346" s="36"/>
     </row>
     <row r="347" ht="14.25" customHeight="1">
-      <c r="K347" s="37"/>
+      <c r="K347" s="36"/>
     </row>
     <row r="348" ht="14.25" customHeight="1">
-      <c r="K348" s="37"/>
+      <c r="K348" s="36"/>
     </row>
     <row r="349" ht="14.25" customHeight="1">
-      <c r="K349" s="37"/>
+      <c r="K349" s="36"/>
     </row>
     <row r="350" ht="14.25" customHeight="1">
-      <c r="K350" s="37"/>
+      <c r="K350" s="36"/>
     </row>
     <row r="351" ht="14.25" customHeight="1">
-      <c r="K351" s="37"/>
+      <c r="K351" s="36"/>
     </row>
     <row r="352" ht="14.25" customHeight="1">
-      <c r="K352" s="37"/>
+      <c r="K352" s="36"/>
     </row>
     <row r="353" ht="14.25" customHeight="1">
-      <c r="K353" s="37"/>
+      <c r="K353" s="36"/>
     </row>
     <row r="354" ht="14.25" customHeight="1">
-      <c r="K354" s="37"/>
+      <c r="K354" s="36"/>
     </row>
     <row r="355" ht="14.25" customHeight="1">
-      <c r="K355" s="37"/>
+      <c r="K355" s="36"/>
     </row>
     <row r="356" ht="14.25" customHeight="1">
-      <c r="K356" s="37"/>
+      <c r="K356" s="36"/>
     </row>
     <row r="357" ht="14.25" customHeight="1">
-      <c r="K357" s="37"/>
+      <c r="K357" s="36"/>
     </row>
     <row r="358" ht="14.25" customHeight="1">
-      <c r="K358" s="37"/>
+      <c r="K358" s="36"/>
     </row>
     <row r="359" ht="14.25" customHeight="1">
-      <c r="K359" s="37"/>
+      <c r="K359" s="36"/>
     </row>
     <row r="360" ht="14.25" customHeight="1">
-      <c r="K360" s="37"/>
+      <c r="K360" s="36"/>
     </row>
     <row r="361" ht="14.25" customHeight="1">
-      <c r="K361" s="37"/>
+      <c r="K361" s="36"/>
     </row>
     <row r="362" ht="14.25" customHeight="1">
-      <c r="K362" s="37"/>
+      <c r="K362" s="36"/>
     </row>
     <row r="363" ht="14.25" customHeight="1">
-      <c r="K363" s="37"/>
+      <c r="K363" s="36"/>
     </row>
     <row r="364" ht="14.25" customHeight="1">
-      <c r="K364" s="37"/>
+      <c r="K364" s="36"/>
     </row>
     <row r="365" ht="14.25" customHeight="1">
-      <c r="K365" s="37"/>
+      <c r="K365" s="36"/>
     </row>
     <row r="366" ht="14.25" customHeight="1">
-      <c r="K366" s="37"/>
+      <c r="K366" s="36"/>
     </row>
     <row r="367" ht="14.25" customHeight="1">
-      <c r="K367" s="37"/>
+      <c r="K367" s="36"/>
     </row>
     <row r="368" ht="14.25" customHeight="1">
-      <c r="K368" s="37"/>
+      <c r="K368" s="36"/>
     </row>
     <row r="369" ht="14.25" customHeight="1">
-      <c r="K369" s="37"/>
+      <c r="K369" s="36"/>
     </row>
     <row r="370" ht="14.25" customHeight="1">
-      <c r="K370" s="37"/>
+      <c r="K370" s="36"/>
     </row>
     <row r="371" ht="14.25" customHeight="1">
-      <c r="K371" s="37"/>
+      <c r="K371" s="36"/>
     </row>
     <row r="372" ht="14.25" customHeight="1">
-      <c r="K372" s="37"/>
+      <c r="K372" s="36"/>
     </row>
     <row r="373" ht="14.25" customHeight="1">
-      <c r="K373" s="37"/>
+      <c r="K373" s="36"/>
     </row>
     <row r="374" ht="14.25" customHeight="1">
-      <c r="K374" s="37"/>
+      <c r="K374" s="36"/>
     </row>
     <row r="375" ht="14.25" customHeight="1">
-      <c r="K375" s="37"/>
+      <c r="K375" s="36"/>
     </row>
     <row r="376" ht="14.25" customHeight="1">
-      <c r="K376" s="37"/>
+      <c r="K376" s="36"/>
     </row>
     <row r="377" ht="14.25" customHeight="1">
-      <c r="K377" s="37"/>
+      <c r="K377" s="36"/>
     </row>
     <row r="378" ht="14.25" customHeight="1">
-      <c r="K378" s="37"/>
+      <c r="K378" s="36"/>
     </row>
     <row r="379" ht="14.25" customHeight="1">
-      <c r="K379" s="37"/>
+      <c r="K379" s="36"/>
     </row>
     <row r="380" ht="14.25" customHeight="1">
-      <c r="K380" s="37"/>
+      <c r="K380" s="36"/>
     </row>
     <row r="381" ht="14.25" customHeight="1">
-      <c r="K381" s="37"/>
+      <c r="K381" s="36"/>
     </row>
     <row r="382" ht="14.25" customHeight="1">
-      <c r="K382" s="37"/>
+      <c r="K382" s="36"/>
     </row>
     <row r="383" ht="14.25" customHeight="1">
-      <c r="K383" s="37"/>
+      <c r="K383" s="36"/>
     </row>
     <row r="384" ht="14.25" customHeight="1">
-      <c r="K384" s="37"/>
+      <c r="K384" s="36"/>
     </row>
     <row r="385" ht="14.25" customHeight="1">
-      <c r="K385" s="37"/>
+      <c r="K385" s="36"/>
     </row>
     <row r="386" ht="14.25" customHeight="1">
-      <c r="K386" s="37"/>
+      <c r="K386" s="36"/>
     </row>
     <row r="387" ht="14.25" customHeight="1">
-      <c r="K387" s="37"/>
+      <c r="K387" s="36"/>
     </row>
     <row r="388" ht="14.25" customHeight="1">
-      <c r="K388" s="37"/>
+      <c r="K388" s="36"/>
     </row>
     <row r="389" ht="14.25" customHeight="1">
-      <c r="K389" s="37"/>
+      <c r="K389" s="36"/>
     </row>
     <row r="390" ht="14.25" customHeight="1">
-      <c r="K390" s="37"/>
+      <c r="K390" s="36"/>
     </row>
     <row r="391" ht="14.25" customHeight="1">
-      <c r="K391" s="37"/>
+      <c r="K391" s="36"/>
     </row>
     <row r="392" ht="14.25" customHeight="1">
-      <c r="K392" s="37"/>
+      <c r="K392" s="36"/>
     </row>
     <row r="393" ht="14.25" customHeight="1">
-      <c r="K393" s="37"/>
+      <c r="K393" s="36"/>
     </row>
     <row r="394" ht="14.25" customHeight="1">
-      <c r="K394" s="37"/>
+      <c r="K394" s="36"/>
     </row>
     <row r="395" ht="14.25" customHeight="1">
-      <c r="K395" s="37"/>
+      <c r="K395" s="36"/>
     </row>
     <row r="396" ht="14.25" customHeight="1">
-      <c r="K396" s="37"/>
+      <c r="K396" s="36"/>
     </row>
     <row r="397" ht="14.25" customHeight="1">
-      <c r="K397" s="37"/>
+      <c r="K397" s="36"/>
     </row>
     <row r="398" ht="14.25" customHeight="1">
-      <c r="K398" s="37"/>
+      <c r="K398" s="36"/>
     </row>
     <row r="399" ht="14.25" customHeight="1">
-      <c r="K399" s="37"/>
+      <c r="K399" s="36"/>
     </row>
     <row r="400" ht="14.25" customHeight="1">
-      <c r="K400" s="37"/>
+      <c r="K400" s="36"/>
     </row>
     <row r="401" ht="14.25" customHeight="1">
-      <c r="K401" s="37"/>
+      <c r="K401" s="36"/>
     </row>
     <row r="402" ht="14.25" customHeight="1">
-      <c r="K402" s="37"/>
+      <c r="K402" s="36"/>
     </row>
     <row r="403" ht="14.25" customHeight="1">
-      <c r="K403" s="37"/>
+      <c r="K403" s="36"/>
     </row>
     <row r="404" ht="14.25" customHeight="1">
-      <c r="K404" s="37"/>
+      <c r="K404" s="36"/>
     </row>
     <row r="405" ht="14.25" customHeight="1">
-      <c r="K405" s="37"/>
+      <c r="K405" s="36"/>
     </row>
     <row r="406" ht="14.25" customHeight="1">
-      <c r="K406" s="37"/>
+      <c r="K406" s="36"/>
     </row>
     <row r="407" ht="14.25" customHeight="1">
-      <c r="K407" s="37"/>
+      <c r="K407" s="36"/>
     </row>
     <row r="408" ht="14.25" customHeight="1">
-      <c r="K408" s="37"/>
+      <c r="K408" s="36"/>
     </row>
     <row r="409" ht="14.25" customHeight="1">
-      <c r="K409" s="37"/>
+      <c r="K409" s="36"/>
     </row>
     <row r="410" ht="14.25" customHeight="1">
-      <c r="K410" s="37"/>
+      <c r="K410" s="36"/>
     </row>
     <row r="411" ht="14.25" customHeight="1">
-      <c r="K411" s="37"/>
+      <c r="K411" s="36"/>
     </row>
     <row r="412" ht="14.25" customHeight="1">
-      <c r="K412" s="37"/>
+      <c r="K412" s="36"/>
     </row>
     <row r="413" ht="14.25" customHeight="1">
-      <c r="K413" s="37"/>
+      <c r="K413" s="36"/>
     </row>
     <row r="414" ht="14.25" customHeight="1">
-      <c r="K414" s="37"/>
+      <c r="K414" s="36"/>
     </row>
     <row r="415" ht="14.25" customHeight="1">
-      <c r="K415" s="37"/>
+      <c r="K415" s="36"/>
     </row>
     <row r="416" ht="14.25" customHeight="1">
-      <c r="K416" s="37"/>
+      <c r="K416" s="36"/>
     </row>
     <row r="417" ht="14.25" customHeight="1">
-      <c r="K417" s="37"/>
+      <c r="K417" s="36"/>
     </row>
     <row r="418" ht="14.25" customHeight="1">
-      <c r="K418" s="37"/>
+      <c r="K418" s="36"/>
     </row>
     <row r="419" ht="14.25" customHeight="1">
-      <c r="K419" s="37"/>
+      <c r="K419" s="36"/>
     </row>
     <row r="420" ht="14.25" customHeight="1">
-      <c r="K420" s="37"/>
+      <c r="K420" s="36"/>
     </row>
     <row r="421" ht="14.25" customHeight="1">
-      <c r="K421" s="37"/>
+      <c r="K421" s="36"/>
     </row>
     <row r="422" ht="14.25" customHeight="1">
-      <c r="K422" s="37"/>
+      <c r="K422" s="36"/>
     </row>
     <row r="423" ht="14.25" customHeight="1">
-      <c r="K423" s="37"/>
+      <c r="K423" s="36"/>
     </row>
     <row r="424" ht="14.25" customHeight="1">
-      <c r="K424" s="37"/>
+      <c r="K424" s="36"/>
     </row>
     <row r="425" ht="14.25" customHeight="1">
-      <c r="K425" s="37"/>
+      <c r="K425" s="36"/>
     </row>
     <row r="426" ht="14.25" customHeight="1">
-      <c r="K426" s="37"/>
+      <c r="K426" s="36"/>
     </row>
     <row r="427" ht="14.25" customHeight="1">
-      <c r="K427" s="37"/>
+      <c r="K427" s="36"/>
     </row>
     <row r="428" ht="14.25" customHeight="1">
-      <c r="K428" s="37"/>
+      <c r="K428" s="36"/>
     </row>
     <row r="429" ht="14.25" customHeight="1">
-      <c r="K429" s="37"/>
+      <c r="K429" s="36"/>
     </row>
     <row r="430" ht="14.25" customHeight="1">
-      <c r="K430" s="37"/>
+      <c r="K430" s="36"/>
     </row>
     <row r="431" ht="14.25" customHeight="1">
-      <c r="K431" s="37"/>
+      <c r="K431" s="36"/>
     </row>
     <row r="432" ht="14.25" customHeight="1">
-      <c r="K432" s="37"/>
+      <c r="K432" s="36"/>
     </row>
     <row r="433" ht="14.25" customHeight="1">
-      <c r="K433" s="37"/>
+      <c r="K433" s="36"/>
     </row>
     <row r="434" ht="14.25" customHeight="1">
-      <c r="K434" s="37"/>
+      <c r="K434" s="36"/>
     </row>
     <row r="435" ht="14.25" customHeight="1">
-      <c r="K435" s="37"/>
+      <c r="K435" s="36"/>
     </row>
     <row r="436" ht="14.25" customHeight="1">
-      <c r="K436" s="37"/>
+      <c r="K436" s="36"/>
     </row>
     <row r="437" ht="14.25" customHeight="1">
-      <c r="K437" s="37"/>
+      <c r="K437" s="36"/>
     </row>
     <row r="438" ht="14.25" customHeight="1">
-      <c r="K438" s="37"/>
+      <c r="K438" s="36"/>
     </row>
     <row r="439" ht="14.25" customHeight="1">
-      <c r="K439" s="37"/>
+      <c r="K439" s="36"/>
     </row>
     <row r="440" ht="14.25" customHeight="1">
-      <c r="K440" s="37"/>
+      <c r="K440" s="36"/>
     </row>
     <row r="441" ht="14.25" customHeight="1">
-      <c r="K441" s="37"/>
+      <c r="K441" s="36"/>
     </row>
     <row r="442" ht="14.25" customHeight="1">
-      <c r="K442" s="37"/>
+      <c r="K442" s="36"/>
     </row>
     <row r="443" ht="14.25" customHeight="1">
-      <c r="K443" s="37"/>
+      <c r="K443" s="36"/>
     </row>
     <row r="444" ht="14.25" customHeight="1">
-      <c r="K444" s="37"/>
+      <c r="K444" s="36"/>
     </row>
     <row r="445" ht="14.25" customHeight="1">
-      <c r="K445" s="37"/>
+      <c r="K445" s="36"/>
     </row>
     <row r="446" ht="14.25" customHeight="1">
-      <c r="K446" s="37"/>
+      <c r="K446" s="36"/>
     </row>
     <row r="447" ht="14.25" customHeight="1">
-      <c r="K447" s="37"/>
+      <c r="K447" s="36"/>
     </row>
     <row r="448" ht="14.25" customHeight="1">
-      <c r="K448" s="37"/>
+      <c r="K448" s="36"/>
     </row>
     <row r="449" ht="14.25" customHeight="1">
-      <c r="K449" s="37"/>
+      <c r="K449" s="36"/>
     </row>
     <row r="450" ht="14.25" customHeight="1">
-      <c r="K450" s="37"/>
+      <c r="K450" s="36"/>
     </row>
     <row r="451" ht="14.25" customHeight="1">
-      <c r="K451" s="37"/>
+      <c r="K451" s="36"/>
     </row>
     <row r="452" ht="14.25" customHeight="1">
-      <c r="K452" s="37"/>
+      <c r="K452" s="36"/>
     </row>
     <row r="453" ht="14.25" customHeight="1">
-      <c r="K453" s="37"/>
+      <c r="K453" s="36"/>
     </row>
     <row r="454" ht="14.25" customHeight="1">
-      <c r="K454" s="37"/>
+      <c r="K454" s="36"/>
     </row>
     <row r="455" ht="14.25" customHeight="1">
-      <c r="K455" s="37"/>
+      <c r="K455" s="36"/>
     </row>
     <row r="456" ht="14.25" customHeight="1">
-      <c r="K456" s="37"/>
+      <c r="K456" s="36"/>
     </row>
     <row r="457" ht="14.25" customHeight="1">
-      <c r="K457" s="37"/>
+      <c r="K457" s="36"/>
     </row>
     <row r="458" ht="14.25" customHeight="1">
-      <c r="K458" s="37"/>
+      <c r="K458" s="36"/>
     </row>
     <row r="459" ht="14.25" customHeight="1">
-      <c r="K459" s="37"/>
+      <c r="K459" s="36"/>
     </row>
     <row r="460" ht="14.25" customHeight="1">
-      <c r="K460" s="37"/>
+      <c r="K460" s="36"/>
     </row>
     <row r="461" ht="14.25" customHeight="1">
-      <c r="K461" s="37"/>
+      <c r="K461" s="36"/>
     </row>
     <row r="462" ht="14.25" customHeight="1">
-      <c r="K462" s="37"/>
+      <c r="K462" s="36"/>
     </row>
     <row r="463" ht="14.25" customHeight="1">
-      <c r="K463" s="37"/>
+      <c r="K463" s="36"/>
     </row>
     <row r="464" ht="14.25" customHeight="1">
-      <c r="K464" s="37"/>
+      <c r="K464" s="36"/>
     </row>
     <row r="465" ht="14.25" customHeight="1">
-      <c r="K465" s="37"/>
+      <c r="K465" s="36"/>
     </row>
     <row r="466" ht="14.25" customHeight="1">
-      <c r="K466" s="37"/>
+      <c r="K466" s="36"/>
     </row>
     <row r="467" ht="14.25" customHeight="1">
-      <c r="K467" s="37"/>
+      <c r="K467" s="36"/>
     </row>
     <row r="468" ht="14.25" customHeight="1">
-      <c r="K468" s="37"/>
+      <c r="K468" s="36"/>
     </row>
     <row r="469" ht="14.25" customHeight="1">
-      <c r="K469" s="37"/>
+      <c r="K469" s="36"/>
     </row>
     <row r="470" ht="14.25" customHeight="1">
-      <c r="K470" s="37"/>
+      <c r="K470" s="36"/>
     </row>
     <row r="471" ht="14.25" customHeight="1">
-      <c r="K471" s="37"/>
+      <c r="K471" s="36"/>
     </row>
     <row r="472" ht="14.25" customHeight="1">
-      <c r="K472" s="37"/>
+      <c r="K472" s="36"/>
     </row>
     <row r="473" ht="14.25" customHeight="1">
-      <c r="K473" s="37"/>
+      <c r="K473" s="36"/>
     </row>
     <row r="474" ht="14.25" customHeight="1">
-      <c r="K474" s="37"/>
+      <c r="K474" s="36"/>
     </row>
     <row r="475" ht="14.25" customHeight="1">
-      <c r="K475" s="37"/>
+      <c r="K475" s="36"/>
     </row>
     <row r="476" ht="14.25" customHeight="1">
-      <c r="K476" s="37"/>
+      <c r="K476" s="36"/>
     </row>
     <row r="477" ht="14.25" customHeight="1">
-      <c r="K477" s="37"/>
+      <c r="K477" s="36"/>
     </row>
     <row r="478" ht="14.25" customHeight="1">
-      <c r="K478" s="37"/>
+      <c r="K478" s="36"/>
     </row>
     <row r="479" ht="14.25" customHeight="1">
-      <c r="K479" s="37"/>
+      <c r="K479" s="36"/>
     </row>
     <row r="480" ht="14.25" customHeight="1">
-      <c r="K480" s="37"/>
+      <c r="K480" s="36"/>
     </row>
     <row r="481" ht="14.25" customHeight="1">
-      <c r="K481" s="37"/>
+      <c r="K481" s="36"/>
     </row>
     <row r="482" ht="14.25" customHeight="1">
-      <c r="K482" s="37"/>
+      <c r="K482" s="36"/>
     </row>
     <row r="483" ht="14.25" customHeight="1">
-      <c r="K483" s="37"/>
+      <c r="K483" s="36"/>
     </row>
     <row r="484" ht="14.25" customHeight="1">
-      <c r="K484" s="37"/>
+      <c r="K484" s="36"/>
     </row>
     <row r="485" ht="14.25" customHeight="1">
-      <c r="K485" s="37"/>
+      <c r="K485" s="36"/>
     </row>
     <row r="486" ht="14.25" customHeight="1">
-      <c r="K486" s="37"/>
+      <c r="K486" s="36"/>
     </row>
     <row r="487" ht="14.25" customHeight="1">
-      <c r="K487" s="37"/>
+      <c r="K487" s="36"/>
     </row>
     <row r="488" ht="14.25" customHeight="1">
-      <c r="K488" s="37"/>
+      <c r="K488" s="36"/>
     </row>
     <row r="489" ht="14.25" customHeight="1">
-      <c r="K489" s="37"/>
+      <c r="K489" s="36"/>
     </row>
     <row r="490" ht="14.25" customHeight="1">
-      <c r="K490" s="37"/>
+      <c r="K490" s="36"/>
     </row>
     <row r="491" ht="14.25" customHeight="1">
-      <c r="K491" s="37"/>
+      <c r="K491" s="36"/>
     </row>
     <row r="492" ht="14.25" customHeight="1">
-      <c r="K492" s="37"/>
+      <c r="K492" s="36"/>
     </row>
     <row r="493" ht="14.25" customHeight="1">
-      <c r="K493" s="37"/>
+      <c r="K493" s="36"/>
     </row>
     <row r="494" ht="14.25" customHeight="1">
-      <c r="K494" s="37"/>
+      <c r="K494" s="36"/>
     </row>
     <row r="495" ht="14.25" customHeight="1">
-      <c r="K495" s="37"/>
+      <c r="K495" s="36"/>
     </row>
     <row r="496" ht="14.25" customHeight="1">
-      <c r="K496" s="37"/>
+      <c r="K496" s="36"/>
     </row>
     <row r="497" ht="14.25" customHeight="1">
-      <c r="K497" s="37"/>
+      <c r="K497" s="36"/>
     </row>
     <row r="498" ht="14.25" customHeight="1">
-      <c r="K498" s="37"/>
+      <c r="K498" s="36"/>
     </row>
     <row r="499" ht="14.25" customHeight="1">
-      <c r="K499" s="37"/>
+      <c r="K499" s="36"/>
     </row>
     <row r="500" ht="14.25" customHeight="1">
-      <c r="K500" s="37"/>
+      <c r="K500" s="36"/>
     </row>
     <row r="501" ht="14.25" customHeight="1">
-      <c r="K501" s="37"/>
+      <c r="K501" s="36"/>
     </row>
     <row r="502" ht="14.25" customHeight="1">
-      <c r="K502" s="37"/>
+      <c r="K502" s="36"/>
     </row>
     <row r="503" ht="14.25" customHeight="1">
-      <c r="K503" s="37"/>
+      <c r="K503" s="36"/>
     </row>
     <row r="504" ht="14.25" customHeight="1">
-      <c r="K504" s="37"/>
+      <c r="K504" s="36"/>
     </row>
     <row r="505" ht="14.25" customHeight="1">
-      <c r="K505" s="37"/>
+      <c r="K505" s="36"/>
     </row>
     <row r="506" ht="14.25" customHeight="1">
-      <c r="K506" s="37"/>
+      <c r="K506" s="36"/>
     </row>
     <row r="507" ht="14.25" customHeight="1">
-      <c r="K507" s="37"/>
+      <c r="K507" s="36"/>
     </row>
     <row r="508" ht="14.25" customHeight="1">
-      <c r="K508" s="37"/>
+      <c r="K508" s="36"/>
     </row>
     <row r="509" ht="14.25" customHeight="1">
-      <c r="K509" s="37"/>
+      <c r="K509" s="36"/>
     </row>
     <row r="510" ht="14.25" customHeight="1">
-      <c r="K510" s="37"/>
+      <c r="K510" s="36"/>
     </row>
     <row r="511" ht="14.25" customHeight="1">
-      <c r="K511" s="37"/>
+      <c r="K511" s="36"/>
     </row>
     <row r="512" ht="14.25" customHeight="1">
-      <c r="K512" s="37"/>
+      <c r="K512" s="36"/>
     </row>
     <row r="513" ht="14.25" customHeight="1">
-      <c r="K513" s="37"/>
+      <c r="K513" s="36"/>
     </row>
     <row r="514" ht="14.25" customHeight="1">
-      <c r="K514" s="37"/>
+      <c r="K514" s="36"/>
     </row>
     <row r="515" ht="14.25" customHeight="1">
-      <c r="K515" s="37"/>
+      <c r="K515" s="36"/>
     </row>
     <row r="516" ht="14.25" customHeight="1">
-      <c r="K516" s="37"/>
+      <c r="K516" s="36"/>
     </row>
     <row r="517" ht="14.25" customHeight="1">
-      <c r="K517" s="37"/>
+      <c r="K517" s="36"/>
     </row>
     <row r="518" ht="14.25" customHeight="1">
-      <c r="K518" s="37"/>
+      <c r="K518" s="36"/>
     </row>
     <row r="519" ht="14.25" customHeight="1">
-      <c r="K519" s="37"/>
+      <c r="K519" s="36"/>
     </row>
     <row r="520" ht="14.25" customHeight="1">
-      <c r="K520" s="37"/>
+      <c r="K520" s="36"/>
     </row>
     <row r="521" ht="14.25" customHeight="1">
-      <c r="K521" s="37"/>
+      <c r="K521" s="36"/>
     </row>
     <row r="522" ht="14.25" customHeight="1">
-      <c r="K522" s="37"/>
+      <c r="K522" s="36"/>
     </row>
     <row r="523" ht="14.25" customHeight="1">
-      <c r="K523" s="37"/>
+      <c r="K523" s="36"/>
     </row>
     <row r="524" ht="14.25" customHeight="1">
-      <c r="K524" s="37"/>
+      <c r="K524" s="36"/>
     </row>
     <row r="525" ht="14.25" customHeight="1">
-      <c r="K525" s="37"/>
+      <c r="K525" s="36"/>
     </row>
     <row r="526" ht="14.25" customHeight="1">
-      <c r="K526" s="37"/>
+      <c r="K526" s="36"/>
     </row>
     <row r="527" ht="14.25" customHeight="1">
-      <c r="K527" s="37"/>
+      <c r="K527" s="36"/>
     </row>
     <row r="528" ht="14.25" customHeight="1">
-      <c r="K528" s="37"/>
+      <c r="K528" s="36"/>
     </row>
     <row r="529" ht="14.25" customHeight="1">
-      <c r="K529" s="37"/>
+      <c r="K529" s="36"/>
     </row>
     <row r="530" ht="14.25" customHeight="1">
-      <c r="K530" s="37"/>
+      <c r="K530" s="36"/>
     </row>
     <row r="531" ht="14.25" customHeight="1">
-      <c r="K531" s="37"/>
+      <c r="K531" s="36"/>
     </row>
     <row r="532" ht="14.25" customHeight="1">
-      <c r="K532" s="37"/>
+      <c r="K532" s="36"/>
     </row>
     <row r="533" ht="14.25" customHeight="1">
-      <c r="K533" s="37"/>
+      <c r="K533" s="36"/>
     </row>
     <row r="534" ht="14.25" customHeight="1">
-      <c r="K534" s="37"/>
+      <c r="K534" s="36"/>
     </row>
     <row r="535" ht="14.25" customHeight="1">
-      <c r="K535" s="37"/>
+      <c r="K535" s="36"/>
     </row>
     <row r="536" ht="14.25" customHeight="1">
-      <c r="K536" s="37"/>
+      <c r="K536" s="36"/>
     </row>
     <row r="537" ht="14.25" customHeight="1">
-      <c r="K537" s="37"/>
+      <c r="K537" s="36"/>
     </row>
     <row r="538" ht="14.25" customHeight="1">
-      <c r="K538" s="37"/>
+      <c r="K538" s="36"/>
     </row>
     <row r="539" ht="14.25" customHeight="1">
-      <c r="K539" s="37"/>
+      <c r="K539" s="36"/>
     </row>
     <row r="540" ht="14.25" customHeight="1">
-      <c r="K540" s="37"/>
+      <c r="K540" s="36"/>
     </row>
     <row r="541" ht="14.25" customHeight="1">
-      <c r="K541" s="37"/>
+      <c r="K541" s="36"/>
     </row>
     <row r="542" ht="14.25" customHeight="1">
-      <c r="K542" s="37"/>
+      <c r="K542" s="36"/>
     </row>
     <row r="543" ht="14.25" customHeight="1">
-      <c r="K543" s="37"/>
+      <c r="K543" s="36"/>
     </row>
     <row r="544" ht="14.25" customHeight="1">
-      <c r="K544" s="37"/>
+      <c r="K544" s="36"/>
     </row>
     <row r="545" ht="14.25" customHeight="1">
-      <c r="K545" s="37"/>
+      <c r="K545" s="36"/>
     </row>
     <row r="546" ht="14.25" customHeight="1">
-      <c r="K546" s="37"/>
+      <c r="K546" s="36"/>
     </row>
     <row r="547" ht="14.25" customHeight="1">
-      <c r="K547" s="37"/>
+      <c r="K547" s="36"/>
     </row>
     <row r="548" ht="14.25" customHeight="1">
-      <c r="K548" s="37"/>
+      <c r="K548" s="36"/>
     </row>
     <row r="549" ht="14.25" customHeight="1">
-      <c r="K549" s="37"/>
+      <c r="K549" s="36"/>
     </row>
     <row r="550" ht="14.25" customHeight="1">
-      <c r="K550" s="37"/>
+      <c r="K550" s="36"/>
     </row>
     <row r="551" ht="14.25" customHeight="1">
-      <c r="K551" s="37"/>
+      <c r="K551" s="36"/>
     </row>
     <row r="552" ht="14.25" customHeight="1">
-      <c r="K552" s="37"/>
+      <c r="K552" s="36"/>
     </row>
     <row r="553" ht="14.25" customHeight="1">
-      <c r="K553" s="37"/>
+      <c r="K553" s="36"/>
     </row>
     <row r="554" ht="14.25" customHeight="1">
-      <c r="K554" s="37"/>
+      <c r="K554" s="36"/>
     </row>
     <row r="555" ht="14.25" customHeight="1">
-      <c r="K555" s="37"/>
+      <c r="K555" s="36"/>
     </row>
     <row r="556" ht="14.25" customHeight="1">
-      <c r="K556" s="37"/>
+      <c r="K556" s="36"/>
     </row>
     <row r="557" ht="14.25" customHeight="1">
-      <c r="K557" s="37"/>
+      <c r="K557" s="36"/>
     </row>
     <row r="558" ht="14.25" customHeight="1">
-      <c r="K558" s="37"/>
+      <c r="K558" s="36"/>
     </row>
     <row r="559" ht="14.25" customHeight="1">
-      <c r="K559" s="37"/>
+      <c r="K559" s="36"/>
     </row>
     <row r="560" ht="14.25" customHeight="1">
-      <c r="K560" s="37"/>
+      <c r="K560" s="36"/>
     </row>
     <row r="561" ht="14.25" customHeight="1">
-      <c r="K561" s="37"/>
+      <c r="K561" s="36"/>
     </row>
     <row r="562" ht="14.25" customHeight="1">
-      <c r="K562" s="37"/>
+      <c r="K562" s="36"/>
     </row>
     <row r="563" ht="14.25" customHeight="1">
-      <c r="K563" s="37"/>
+      <c r="K563" s="36"/>
     </row>
     <row r="564" ht="14.25" customHeight="1">
-      <c r="K564" s="37"/>
+      <c r="K564" s="36"/>
     </row>
     <row r="565" ht="14.25" customHeight="1">
-      <c r="K565" s="37"/>
+      <c r="K565" s="36"/>
     </row>
     <row r="566" ht="14.25" customHeight="1">
-      <c r="K566" s="37"/>
+      <c r="K566" s="36"/>
     </row>
     <row r="567" ht="14.25" customHeight="1">
-      <c r="K567" s="37"/>
+      <c r="K567" s="36"/>
     </row>
     <row r="568" ht="14.25" customHeight="1">
-      <c r="K568" s="37"/>
+      <c r="K568" s="36"/>
     </row>
     <row r="569" ht="14.25" customHeight="1">
-      <c r="K569" s="37"/>
+      <c r="K569" s="36"/>
     </row>
     <row r="570" ht="14.25" customHeight="1">
-      <c r="K570" s="37"/>
+      <c r="K570" s="36"/>
     </row>
     <row r="571" ht="14.25" customHeight="1">
-      <c r="K571" s="37"/>
+      <c r="K571" s="36"/>
     </row>
     <row r="572" ht="14.25" customHeight="1">
-      <c r="K572" s="37"/>
+      <c r="K572" s="36"/>
     </row>
     <row r="573" ht="14.25" customHeight="1">
-      <c r="K573" s="37"/>
+      <c r="K573" s="36"/>
     </row>
     <row r="574" ht="14.25" customHeight="1">
-      <c r="K574" s="37"/>
+      <c r="K574" s="36"/>
     </row>
     <row r="575" ht="14.25" customHeight="1">
-      <c r="K575" s="37"/>
+      <c r="K575" s="36"/>
     </row>
     <row r="576" ht="14.25" customHeight="1">
-      <c r="K576" s="37"/>
+      <c r="K576" s="36"/>
     </row>
     <row r="577" ht="14.25" customHeight="1">
-      <c r="K577" s="37"/>
+      <c r="K577" s="36"/>
     </row>
     <row r="578" ht="14.25" customHeight="1">
-      <c r="K578" s="37"/>
+      <c r="K578" s="36"/>
     </row>
     <row r="579" ht="14.25" customHeight="1">
-      <c r="K579" s="37"/>
+      <c r="K579" s="36"/>
     </row>
     <row r="580" ht="14.25" customHeight="1">
-      <c r="K580" s="37"/>
+      <c r="K580" s="36"/>
     </row>
     <row r="581" ht="14.25" customHeight="1">
-      <c r="K581" s="37"/>
+      <c r="K581" s="36"/>
     </row>
     <row r="582" ht="14.25" customHeight="1">
-      <c r="K582" s="37"/>
+      <c r="K582" s="36"/>
     </row>
     <row r="583" ht="14.25" customHeight="1">
-      <c r="K583" s="37"/>
+      <c r="K583" s="36"/>
     </row>
     <row r="584" ht="14.25" customHeight="1">
-      <c r="K584" s="37"/>
+      <c r="K584" s="36"/>
     </row>
     <row r="585" ht="14.25" customHeight="1">
-      <c r="K585" s="37"/>
+      <c r="K585" s="36"/>
     </row>
     <row r="586" ht="14.25" customHeight="1">
-      <c r="K586" s="37"/>
+      <c r="K586" s="36"/>
     </row>
     <row r="587" ht="14.25" customHeight="1">
-      <c r="K587" s="37"/>
+      <c r="K587" s="36"/>
     </row>
     <row r="588" ht="14.25" customHeight="1">
-      <c r="K588" s="37"/>
+      <c r="K588" s="36"/>
     </row>
     <row r="589" ht="14.25" customHeight="1">
-      <c r="K589" s="37"/>
+      <c r="K589" s="36"/>
     </row>
     <row r="590" ht="14.25" customHeight="1">
-      <c r="K590" s="37"/>
+      <c r="K590" s="36"/>
     </row>
     <row r="591" ht="14.25" customHeight="1">
-      <c r="K591" s="37"/>
+      <c r="K591" s="36"/>
     </row>
     <row r="592" ht="14.25" customHeight="1">
-      <c r="K592" s="37"/>
+      <c r="K592" s="36"/>
     </row>
     <row r="593" ht="14.25" customHeight="1">
-      <c r="K593" s="37"/>
+      <c r="K593" s="36"/>
     </row>
     <row r="594" ht="14.25" customHeight="1">
-      <c r="K594" s="37"/>
+      <c r="K594" s="36"/>
     </row>
     <row r="595" ht="14.25" customHeight="1">
-      <c r="K595" s="37"/>
+      <c r="K595" s="36"/>
     </row>
     <row r="596" ht="14.25" customHeight="1">
-      <c r="K596" s="37"/>
+      <c r="K596" s="36"/>
     </row>
     <row r="597" ht="14.25" customHeight="1">
-      <c r="K597" s="37"/>
+      <c r="K597" s="36"/>
     </row>
     <row r="598" ht="14.25" customHeight="1">
-      <c r="K598" s="37"/>
+      <c r="K598" s="36"/>
     </row>
     <row r="599" ht="14.25" customHeight="1">
-      <c r="K599" s="37"/>
+      <c r="K599" s="36"/>
     </row>
     <row r="600" ht="14.25" customHeight="1">
-      <c r="K600" s="37"/>
+      <c r="K600" s="36"/>
     </row>
     <row r="601" ht="14.25" customHeight="1">
-      <c r="K601" s="37"/>
+      <c r="K601" s="36"/>
     </row>
     <row r="602" ht="14.25" customHeight="1">
-      <c r="K602" s="37"/>
+      <c r="K602" s="36"/>
     </row>
     <row r="603" ht="14.25" customHeight="1">
-      <c r="K603" s="37"/>
+      <c r="K603" s="36"/>
     </row>
     <row r="604" ht="14.25" customHeight="1">
-      <c r="K604" s="37"/>
+      <c r="K604" s="36"/>
     </row>
     <row r="605" ht="14.25" customHeight="1">
-      <c r="K605" s="37"/>
+      <c r="K605" s="36"/>
     </row>
     <row r="606" ht="14.25" customHeight="1">
-      <c r="K606" s="37"/>
+      <c r="K606" s="36"/>
     </row>
     <row r="607" ht="14.25" customHeight="1">
-      <c r="K607" s="37"/>
+      <c r="K607" s="36"/>
     </row>
     <row r="608" ht="14.25" customHeight="1">
-      <c r="K608" s="37"/>
+      <c r="K608" s="36"/>
     </row>
     <row r="609" ht="14.25" customHeight="1">
-      <c r="K609" s="37"/>
+      <c r="K609" s="36"/>
     </row>
     <row r="610" ht="14.25" customHeight="1">
-      <c r="K610" s="37"/>
+      <c r="K610" s="36"/>
     </row>
     <row r="611" ht="14.25" customHeight="1">
-      <c r="K611" s="37"/>
+      <c r="K611" s="36"/>
     </row>
     <row r="612" ht="14.25" customHeight="1">
-      <c r="K612" s="37"/>
+      <c r="K612" s="36"/>
     </row>
     <row r="613" ht="14.25" customHeight="1">
-      <c r="K613" s="37"/>
+      <c r="K613" s="36"/>
     </row>
     <row r="614" ht="14.25" customHeight="1">
-      <c r="K614" s="37"/>
+      <c r="K614" s="36"/>
     </row>
     <row r="615" ht="14.25" customHeight="1">
-      <c r="K615" s="37"/>
+      <c r="K615" s="36"/>
     </row>
     <row r="616" ht="14.25" customHeight="1">
-      <c r="K616" s="37"/>
+      <c r="K616" s="36"/>
     </row>
     <row r="617" ht="14.25" customHeight="1">
-      <c r="K617" s="37"/>
+      <c r="K617" s="36"/>
     </row>
     <row r="618" ht="14.25" customHeight="1">
-      <c r="K618" s="37"/>
+      <c r="K618" s="36"/>
     </row>
     <row r="619" ht="14.25" customHeight="1">
-      <c r="K619" s="37"/>
+      <c r="K619" s="36"/>
     </row>
     <row r="620" ht="14.25" customHeight="1">
-      <c r="K620" s="37"/>
+      <c r="K620" s="36"/>
     </row>
     <row r="621" ht="14.25" customHeight="1">
-      <c r="K621" s="37"/>
+      <c r="K621" s="36"/>
     </row>
     <row r="622" ht="14.25" customHeight="1">
-      <c r="K622" s="37"/>
+      <c r="K622" s="36"/>
     </row>
     <row r="623" ht="14.25" customHeight="1">
-      <c r="K623" s="37"/>
+      <c r="K623" s="36"/>
     </row>
     <row r="624" ht="14.25" customHeight="1">
-      <c r="K624" s="37"/>
+      <c r="K624" s="36"/>
     </row>
     <row r="625" ht="14.25" customHeight="1">
-      <c r="K625" s="37"/>
+      <c r="K625" s="36"/>
     </row>
     <row r="626" ht="14.25" customHeight="1">
-      <c r="K626" s="37"/>
+      <c r="K626" s="36"/>
     </row>
     <row r="627" ht="14.25" customHeight="1">
-      <c r="K627" s="37"/>
+      <c r="K627" s="36"/>
     </row>
     <row r="628" ht="14.25" customHeight="1">
-      <c r="K628" s="37"/>
+      <c r="K628" s="36"/>
     </row>
     <row r="629" ht="14.25" customHeight="1">
-      <c r="K629" s="37"/>
+      <c r="K629" s="36"/>
     </row>
     <row r="630" ht="14.25" customHeight="1">
-      <c r="K630" s="37"/>
+      <c r="K630" s="36"/>
     </row>
     <row r="631" ht="14.25" customHeight="1">
-      <c r="K631" s="37"/>
+      <c r="K631" s="36"/>
     </row>
     <row r="632" ht="14.25" customHeight="1">
-      <c r="K632" s="37"/>
+      <c r="K632" s="36"/>
     </row>
     <row r="633" ht="14.25" customHeight="1">
-      <c r="K633" s="37"/>
+      <c r="K633" s="36"/>
     </row>
     <row r="634" ht="14.25" customHeight="1">
-      <c r="K634" s="37"/>
+      <c r="K634" s="36"/>
     </row>
     <row r="635" ht="14.25" customHeight="1">
-      <c r="K635" s="37"/>
+      <c r="K635" s="36"/>
     </row>
     <row r="636" ht="14.25" customHeight="1">
-      <c r="K636" s="37"/>
+      <c r="K636" s="36"/>
     </row>
     <row r="637" ht="14.25" customHeight="1">
-      <c r="K637" s="37"/>
+      <c r="K637" s="36"/>
     </row>
     <row r="638" ht="14.25" customHeight="1">
-      <c r="K638" s="37"/>
+      <c r="K638" s="36"/>
     </row>
     <row r="639" ht="14.25" customHeight="1">
-      <c r="K639" s="37"/>
+      <c r="K639" s="36"/>
     </row>
     <row r="640" ht="14.25" customHeight="1">
-      <c r="K640" s="37"/>
+      <c r="K640" s="36"/>
     </row>
     <row r="641" ht="14.25" customHeight="1">
-      <c r="K641" s="37"/>
+      <c r="K641" s="36"/>
     </row>
     <row r="642" ht="14.25" customHeight="1">
-      <c r="K642" s="37"/>
+      <c r="K642" s="36"/>
     </row>
     <row r="643" ht="14.25" customHeight="1">
-      <c r="K643" s="37"/>
+      <c r="K643" s="36"/>
     </row>
     <row r="644" ht="14.25" customHeight="1">
-      <c r="K644" s="37"/>
+      <c r="K644" s="36"/>
     </row>
     <row r="645" ht="14.25" customHeight="1">
-      <c r="K645" s="37"/>
+      <c r="K645" s="36"/>
     </row>
     <row r="646" ht="14.25" customHeight="1">
-      <c r="K646" s="37"/>
+      <c r="K646" s="36"/>
     </row>
     <row r="647" ht="14.25" customHeight="1">
-      <c r="K647" s="37"/>
+      <c r="K647" s="36"/>
     </row>
     <row r="648" ht="14.25" customHeight="1">
-      <c r="K648" s="37"/>
+      <c r="K648" s="36"/>
     </row>
     <row r="649" ht="14.25" customHeight="1">
-      <c r="K649" s="37"/>
+      <c r="K649" s="36"/>
     </row>
     <row r="650" ht="14.25" customHeight="1">
-      <c r="K650" s="37"/>
+      <c r="K650" s="36"/>
     </row>
     <row r="651" ht="14.25" customHeight="1">
-      <c r="K651" s="37"/>
+      <c r="K651" s="36"/>
     </row>
     <row r="652" ht="14.25" customHeight="1">
-      <c r="K652" s="37"/>
+      <c r="K652" s="36"/>
     </row>
     <row r="653" ht="14.25" customHeight="1">
-      <c r="K653" s="37"/>
+      <c r="K653" s="36"/>
     </row>
     <row r="654" ht="14.25" customHeight="1">
-      <c r="K654" s="37"/>
+      <c r="K654" s="36"/>
     </row>
     <row r="655" ht="14.25" customHeight="1">
-      <c r="K655" s="37"/>
+      <c r="K655" s="36"/>
     </row>
     <row r="656" ht="14.25" customHeight="1">
-      <c r="K656" s="37"/>
+      <c r="K656" s="36"/>
     </row>
     <row r="657" ht="14.25" customHeight="1">
-      <c r="K657" s="37"/>
+      <c r="K657" s="36"/>
     </row>
     <row r="658" ht="14.25" customHeight="1">
-      <c r="K658" s="37"/>
+      <c r="K658" s="36"/>
     </row>
     <row r="659" ht="14.25" customHeight="1">
-      <c r="K659" s="37"/>
+      <c r="K659" s="36"/>
     </row>
     <row r="660" ht="14.25" customHeight="1">
-      <c r="K660" s="37"/>
+      <c r="K660" s="36"/>
     </row>
     <row r="661" ht="14.25" customHeight="1">
-      <c r="K661" s="37"/>
+      <c r="K661" s="36"/>
     </row>
     <row r="662" ht="14.25" customHeight="1">
-      <c r="K662" s="37"/>
+      <c r="K662" s="36"/>
     </row>
     <row r="663" ht="14.25" customHeight="1">
-      <c r="K663" s="37"/>
+      <c r="K663" s="36"/>
     </row>
     <row r="664" ht="14.25" customHeight="1">
-      <c r="K664" s="37"/>
+      <c r="K664" s="36"/>
     </row>
     <row r="665" ht="14.25" customHeight="1">
-      <c r="K665" s="37"/>
+      <c r="K665" s="36"/>
     </row>
     <row r="666" ht="14.25" customHeight="1">
-      <c r="K666" s="37"/>
+      <c r="K666" s="36"/>
     </row>
     <row r="667" ht="14.25" customHeight="1">
-      <c r="K667" s="37"/>
+      <c r="K667" s="36"/>
     </row>
     <row r="668" ht="14.25" customHeight="1">
-      <c r="K668" s="37"/>
+      <c r="K668" s="36"/>
     </row>
     <row r="669" ht="14.25" customHeight="1">
-      <c r="K669" s="37"/>
+      <c r="K669" s="36"/>
     </row>
     <row r="670" ht="14.25" customHeight="1">
-      <c r="K670" s="37"/>
+      <c r="K670" s="36"/>
     </row>
     <row r="671" ht="14.25" customHeight="1">
-      <c r="K671" s="37"/>
+      <c r="K671" s="36"/>
     </row>
     <row r="672" ht="14.25" customHeight="1">
-      <c r="K672" s="37"/>
+      <c r="K672" s="36"/>
     </row>
     <row r="673" ht="14.25" customHeight="1">
-      <c r="K673" s="37"/>
+      <c r="K673" s="36"/>
     </row>
     <row r="674" ht="14.25" customHeight="1">
-      <c r="K674" s="37"/>
+      <c r="K674" s="36"/>
     </row>
     <row r="675" ht="14.25" customHeight="1">
-      <c r="K675" s="37"/>
+      <c r="K675" s="36"/>
     </row>
     <row r="676" ht="14.25" customHeight="1">
-      <c r="K676" s="37"/>
+      <c r="K676" s="36"/>
     </row>
     <row r="677" ht="14.25" customHeight="1">
-      <c r="K677" s="37"/>
+      <c r="K677" s="36"/>
     </row>
     <row r="678" ht="14.25" customHeight="1">
-      <c r="K678" s="37"/>
+      <c r="K678" s="36"/>
     </row>
     <row r="679" ht="14.25" customHeight="1">
-      <c r="K679" s="37"/>
+      <c r="K679" s="36"/>
     </row>
     <row r="680" ht="14.25" customHeight="1">
-      <c r="K680" s="37"/>
+      <c r="K680" s="36"/>
     </row>
     <row r="681" ht="14.25" customHeight="1">
-      <c r="K681" s="37"/>
+      <c r="K681" s="36"/>
     </row>
     <row r="682" ht="14.25" customHeight="1">
-      <c r="K682" s="37"/>
+      <c r="K682" s="36"/>
     </row>
     <row r="683" ht="14.25" customHeight="1">
-      <c r="K683" s="37"/>
+      <c r="K683" s="36"/>
     </row>
     <row r="684" ht="14.25" customHeight="1">
-      <c r="K684" s="37"/>
+      <c r="K684" s="36"/>
     </row>
     <row r="685" ht="14.25" customHeight="1">
-      <c r="K685" s="37"/>
+      <c r="K685" s="36"/>
     </row>
     <row r="686" ht="14.25" customHeight="1">
-      <c r="K686" s="37"/>
+      <c r="K686" s="36"/>
     </row>
     <row r="687" ht="14.25" customHeight="1">
-      <c r="K687" s="37"/>
+      <c r="K687" s="36"/>
     </row>
     <row r="688" ht="14.25" customHeight="1">
-      <c r="K688" s="37"/>
+      <c r="K688" s="36"/>
     </row>
     <row r="689" ht="14.25" customHeight="1">
-      <c r="K689" s="37"/>
+      <c r="K689" s="36"/>
     </row>
     <row r="690" ht="14.25" customHeight="1">
-      <c r="K690" s="37"/>
+      <c r="K690" s="36"/>
     </row>
     <row r="691" ht="14.25" customHeight="1">
-      <c r="K691" s="37"/>
+      <c r="K691" s="36"/>
     </row>
     <row r="692" ht="14.25" customHeight="1">
-      <c r="K692" s="37"/>
+      <c r="K692" s="36"/>
     </row>
     <row r="693" ht="14.25" customHeight="1">
-      <c r="K693" s="37"/>
+      <c r="K693" s="36"/>
     </row>
     <row r="694" ht="14.25" customHeight="1">
-      <c r="K694" s="37"/>
+      <c r="K694" s="36"/>
     </row>
     <row r="695" ht="14.25" customHeight="1">
-      <c r="K695" s="37"/>
+      <c r="K695" s="36"/>
     </row>
     <row r="696" ht="14.25" customHeight="1">
-      <c r="K696" s="37"/>
+      <c r="K696" s="36"/>
     </row>
     <row r="697" ht="14.25" customHeight="1">
-      <c r="K697" s="37"/>
+      <c r="K697" s="36"/>
     </row>
     <row r="698" ht="14.25" customHeight="1">
-      <c r="K698" s="37"/>
+      <c r="K698" s="36"/>
     </row>
     <row r="699" ht="14.25" customHeight="1">
-      <c r="K699" s="37"/>
+      <c r="K699" s="36"/>
     </row>
     <row r="700" ht="14.25" customHeight="1">
-      <c r="K700" s="37"/>
+      <c r="K700" s="36"/>
     </row>
     <row r="701" ht="14.25" customHeight="1">
-      <c r="K701" s="37"/>
+      <c r="K701" s="36"/>
     </row>
     <row r="702" ht="14.25" customHeight="1">
-      <c r="K702" s="37"/>
+      <c r="K702" s="36"/>
     </row>
     <row r="703" ht="14.25" customHeight="1">
-      <c r="K703" s="37"/>
+      <c r="K703" s="36"/>
     </row>
     <row r="704" ht="14.25" customHeight="1">
-      <c r="K704" s="37"/>
+      <c r="K704" s="36"/>
     </row>
     <row r="705" ht="14.25" customHeight="1">
-      <c r="K705" s="37"/>
+      <c r="K705" s="36"/>
     </row>
     <row r="706" ht="14.25" customHeight="1">
-      <c r="K706" s="37"/>
+      <c r="K706" s="36"/>
     </row>
     <row r="707" ht="14.25" customHeight="1">
-      <c r="K707" s="37"/>
+      <c r="K707" s="36"/>
     </row>
     <row r="708" ht="14.25" customHeight="1">
-      <c r="K708" s="37"/>
+      <c r="K708" s="36"/>
     </row>
     <row r="709" ht="14.25" customHeight="1">
-      <c r="K709" s="37"/>
+      <c r="K709" s="36"/>
     </row>
     <row r="710" ht="14.25" customHeight="1">
-      <c r="K710" s="37"/>
+      <c r="K710" s="36"/>
     </row>
     <row r="711" ht="14.25" customHeight="1">
-      <c r="K711" s="37"/>
+      <c r="K711" s="36"/>
     </row>
     <row r="712" ht="14.25" customHeight="1">
-      <c r="K712" s="37"/>
+      <c r="K712" s="36"/>
     </row>
     <row r="713" ht="14.25" customHeight="1">
-      <c r="K713" s="37"/>
+      <c r="K713" s="36"/>
     </row>
     <row r="714" ht="14.25" customHeight="1">
-      <c r="K714" s="37"/>
+      <c r="K714" s="36"/>
     </row>
     <row r="715" ht="14.25" customHeight="1">
-      <c r="K715" s="37"/>
+      <c r="K715" s="36"/>
     </row>
     <row r="716" ht="14.25" customHeight="1">
-      <c r="K716" s="37"/>
+      <c r="K716" s="36"/>
     </row>
     <row r="717" ht="14.25" customHeight="1">
-      <c r="K717" s="37"/>
+      <c r="K717" s="36"/>
     </row>
     <row r="718" ht="14.25" customHeight="1">
-      <c r="K718" s="37"/>
+      <c r="K718" s="36"/>
     </row>
     <row r="719" ht="14.25" customHeight="1">
-      <c r="K719" s="37"/>
+      <c r="K719" s="36"/>
     </row>
     <row r="720" ht="14.25" customHeight="1">
-      <c r="K720" s="37"/>
+      <c r="K720" s="36"/>
     </row>
     <row r="721" ht="14.25" customHeight="1">
-      <c r="K721" s="37"/>
+      <c r="K721" s="36"/>
     </row>
     <row r="722" ht="14.25" customHeight="1">
-      <c r="K722" s="37"/>
+      <c r="K722" s="36"/>
     </row>
     <row r="723" ht="14.25" customHeight="1">
-      <c r="K723" s="37"/>
+      <c r="K723" s="36"/>
     </row>
     <row r="724" ht="14.25" customHeight="1">
-      <c r="K724" s="37"/>
+      <c r="K724" s="36"/>
     </row>
     <row r="725" ht="14.25" customHeight="1">
-      <c r="K725" s="37"/>
+      <c r="K725" s="36"/>
     </row>
     <row r="726" ht="14.25" customHeight="1">
-      <c r="K726" s="37"/>
+      <c r="K726" s="36"/>
     </row>
     <row r="727" ht="14.25" customHeight="1">
-      <c r="K727" s="37"/>
+      <c r="K727" s="36"/>
     </row>
     <row r="728" ht="14.25" customHeight="1">
-      <c r="K728" s="37"/>
+      <c r="K728" s="36"/>
     </row>
     <row r="729" ht="14.25" customHeight="1">
-      <c r="K729" s="37"/>
+      <c r="K729" s="36"/>
     </row>
     <row r="730" ht="14.25" customHeight="1">
-      <c r="K730" s="37"/>
+      <c r="K730" s="36"/>
     </row>
     <row r="731" ht="14.25" customHeight="1">
-      <c r="K731" s="37"/>
+      <c r="K731" s="36"/>
     </row>
     <row r="732" ht="14.25" customHeight="1">
-      <c r="K732" s="37"/>
+      <c r="K732" s="36"/>
     </row>
     <row r="733" ht="14.25" customHeight="1">
-      <c r="K733" s="37"/>
+      <c r="K733" s="36"/>
     </row>
     <row r="734" ht="14.25" customHeight="1">
-      <c r="K734" s="37"/>
+      <c r="K734" s="36"/>
     </row>
     <row r="735" ht="14.25" customHeight="1">
-      <c r="K735" s="37"/>
+      <c r="K735" s="36"/>
     </row>
     <row r="736" ht="14.25" customHeight="1">
-      <c r="K736" s="37"/>
+      <c r="K736" s="36"/>
     </row>
     <row r="737" ht="14.25" customHeight="1">
-      <c r="K737" s="37"/>
+      <c r="K737" s="36"/>
     </row>
     <row r="738" ht="14.25" customHeight="1">
-      <c r="K738" s="37"/>
+      <c r="K738" s="36"/>
     </row>
     <row r="739" ht="14.25" customHeight="1">
-      <c r="K739" s="37"/>
+      <c r="K739" s="36"/>
     </row>
     <row r="740" ht="14.25" customHeight="1">
-      <c r="K740" s="37"/>
+      <c r="K740" s="36"/>
     </row>
     <row r="741" ht="14.25" customHeight="1">
-      <c r="K741" s="37"/>
+      <c r="K741" s="36"/>
     </row>
     <row r="742" ht="14.25" customHeight="1">
-      <c r="K742" s="37"/>
+      <c r="K742" s="36"/>
     </row>
     <row r="743" ht="14.25" customHeight="1">
-      <c r="K743" s="37"/>
+      <c r="K743" s="36"/>
     </row>
     <row r="744" ht="14.25" customHeight="1">
-      <c r="K744" s="37"/>
+      <c r="K744" s="36"/>
     </row>
     <row r="745" ht="14.25" customHeight="1">
-      <c r="K745" s="37"/>
+      <c r="K745" s="36"/>
     </row>
     <row r="746" ht="14.25" customHeight="1">
-      <c r="K746" s="37"/>
+      <c r="K746" s="36"/>
     </row>
     <row r="747" ht="14.25" customHeight="1">
-      <c r="K747" s="37"/>
+      <c r="K747" s="36"/>
     </row>
     <row r="748" ht="14.25" customHeight="1">
-      <c r="K748" s="37"/>
+      <c r="K748" s="36"/>
     </row>
     <row r="749" ht="14.25" customHeight="1">
-      <c r="K749" s="37"/>
+      <c r="K749" s="36"/>
     </row>
     <row r="750" ht="14.25" customHeight="1">
-      <c r="K750" s="37"/>
+      <c r="K750" s="36"/>
     </row>
     <row r="751" ht="14.25" customHeight="1">
-      <c r="K751" s="37"/>
+      <c r="K751" s="36"/>
     </row>
     <row r="752" ht="14.25" customHeight="1">
-      <c r="K752" s="37"/>
+      <c r="K752" s="36"/>
     </row>
     <row r="753" ht="14.25" customHeight="1">
-      <c r="K753" s="37"/>
+      <c r="K753" s="36"/>
     </row>
     <row r="754" ht="14.25" customHeight="1">
-      <c r="K754" s="37"/>
+      <c r="K754" s="36"/>
     </row>
     <row r="755" ht="14.25" customHeight="1">
-      <c r="K755" s="37"/>
+      <c r="K755" s="36"/>
     </row>
     <row r="756" ht="14.25" customHeight="1">
-      <c r="K756" s="37"/>
+      <c r="K756" s="36"/>
     </row>
     <row r="757" ht="14.25" customHeight="1">
-      <c r="K757" s="37"/>
+      <c r="K757" s="36"/>
     </row>
     <row r="758" ht="14.25" customHeight="1">
-      <c r="K758" s="37"/>
+      <c r="K758" s="36"/>
     </row>
     <row r="759" ht="14.25" customHeight="1">
-      <c r="K759" s="37"/>
+      <c r="K759" s="36"/>
     </row>
     <row r="760" ht="14.25" customHeight="1">
-      <c r="K760" s="37"/>
+      <c r="K760" s="36"/>
     </row>
     <row r="761" ht="14.25" customHeight="1">
-      <c r="K761" s="37"/>
+      <c r="K761" s="36"/>
     </row>
     <row r="762" ht="14.25" customHeight="1">
-      <c r="K762" s="37"/>
+      <c r="K762" s="36"/>
     </row>
     <row r="763" ht="14.25" customHeight="1">
-      <c r="K763" s="37"/>
+      <c r="K763" s="36"/>
     </row>
     <row r="764" ht="14.25" customHeight="1">
-      <c r="K764" s="37"/>
+      <c r="K764" s="36"/>
     </row>
     <row r="765" ht="14.25" customHeight="1">
-      <c r="K765" s="37"/>
+      <c r="K765" s="36"/>
     </row>
     <row r="766" ht="14.25" customHeight="1">
-      <c r="K766" s="37"/>
+      <c r="K766" s="36"/>
     </row>
     <row r="767" ht="14.25" customHeight="1">
-      <c r="K767" s="37"/>
+      <c r="K767" s="36"/>
     </row>
     <row r="768" ht="14.25" customHeight="1">
-      <c r="K768" s="37"/>
+      <c r="K768" s="36"/>
     </row>
     <row r="769" ht="14.25" customHeight="1">
-      <c r="K769" s="37"/>
+      <c r="K769" s="36"/>
     </row>
     <row r="770" ht="14.25" customHeight="1">
-      <c r="K770" s="37"/>
+      <c r="K770" s="36"/>
     </row>
     <row r="771" ht="14.25" customHeight="1">
-      <c r="K771" s="37"/>
+      <c r="K771" s="36"/>
     </row>
     <row r="772" ht="14.25" customHeight="1">
-      <c r="K772" s="37"/>
+      <c r="K772" s="36"/>
     </row>
     <row r="773" ht="14.25" customHeight="1">
-      <c r="K773" s="37"/>
+      <c r="K773" s="36"/>
     </row>
     <row r="774" ht="14.25" customHeight="1">
-      <c r="K774" s="37"/>
+      <c r="K774" s="36"/>
     </row>
     <row r="775" ht="14.25" customHeight="1">
-      <c r="K775" s="37"/>
+      <c r="K775" s="36"/>
     </row>
     <row r="776" ht="14.25" customHeight="1">
-      <c r="K776" s="37"/>
+      <c r="K776" s="36"/>
     </row>
     <row r="777" ht="14.25" customHeight="1">
-      <c r="K777" s="37"/>
+      <c r="K777" s="36"/>
     </row>
     <row r="778" ht="14.25" customHeight="1">
-      <c r="K778" s="37"/>
+      <c r="K778" s="36"/>
     </row>
     <row r="779" ht="14.25" customHeight="1">
-      <c r="K779" s="37"/>
+      <c r="K779" s="36"/>
     </row>
     <row r="780" ht="14.25" customHeight="1">
-      <c r="K780" s="37"/>
+      <c r="K780" s="36"/>
     </row>
     <row r="781" ht="14.25" customHeight="1">
-      <c r="K781" s="37"/>
+      <c r="K781" s="36"/>
     </row>
     <row r="782" ht="14.25" customHeight="1">
-      <c r="K782" s="37"/>
+      <c r="K782" s="36"/>
     </row>
     <row r="783" ht="14.25" customHeight="1">
-      <c r="K783" s="37"/>
+      <c r="K783" s="36"/>
     </row>
     <row r="784" ht="14.25" customHeight="1">
-      <c r="K784" s="37"/>
+      <c r="K784" s="36"/>
     </row>
     <row r="785" ht="14.25" customHeight="1">
-      <c r="K785" s="37"/>
+      <c r="K785" s="36"/>
     </row>
     <row r="786" ht="14.25" customHeight="1">
-      <c r="K786" s="37"/>
+      <c r="K786" s="36"/>
     </row>
     <row r="787" ht="14.25" customHeight="1">
-      <c r="K787" s="37"/>
+      <c r="K787" s="36"/>
     </row>
     <row r="788" ht="14.25" customHeight="1">
-      <c r="K788" s="37"/>
+      <c r="K788" s="36"/>
     </row>
     <row r="789" ht="14.25" customHeight="1">
-      <c r="K789" s="37"/>
+      <c r="K789" s="36"/>
     </row>
     <row r="790" ht="14.25" customHeight="1">
-      <c r="K790" s="37"/>
+      <c r="K790" s="36"/>
     </row>
     <row r="791" ht="14.25" customHeight="1">
-      <c r="K791" s="37"/>
+      <c r="K791" s="36"/>
     </row>
     <row r="792" ht="14.25" customHeight="1">
-      <c r="K792" s="37"/>
+      <c r="K792" s="36"/>
     </row>
     <row r="793" ht="14.25" customHeight="1">
-      <c r="K793" s="37"/>
+      <c r="K793" s="36"/>
     </row>
     <row r="794" ht="14.25" customHeight="1">
-      <c r="K794" s="37"/>
+      <c r="K794" s="36"/>
     </row>
     <row r="795" ht="14.25" customHeight="1">
-      <c r="K795" s="37"/>
+      <c r="K795" s="36"/>
     </row>
     <row r="796" ht="14.25" customHeight="1">
-      <c r="K796" s="37"/>
+      <c r="K796" s="36"/>
     </row>
     <row r="797" ht="14.25" customHeight="1">
-      <c r="K797" s="37"/>
+      <c r="K797" s="36"/>
     </row>
     <row r="798" ht="14.25" customHeight="1">
-      <c r="K798" s="37"/>
+      <c r="K798" s="36"/>
     </row>
     <row r="799" ht="14.25" customHeight="1">
-      <c r="K799" s="37"/>
+      <c r="K799" s="36"/>
     </row>
     <row r="800" ht="14.25" customHeight="1">
-      <c r="K800" s="37"/>
+      <c r="K800" s="36"/>
     </row>
     <row r="801" ht="14.25" customHeight="1">
-      <c r="K801" s="37"/>
+      <c r="K801" s="36"/>
     </row>
     <row r="802" ht="14.25" customHeight="1">
-      <c r="K802" s="37"/>
+      <c r="K802" s="36"/>
     </row>
     <row r="803" ht="14.25" customHeight="1">
-      <c r="K803" s="37"/>
+      <c r="K803" s="36"/>
     </row>
     <row r="804" ht="14.25" customHeight="1">
-      <c r="K804" s="37"/>
+      <c r="K804" s="36"/>
     </row>
     <row r="805" ht="14.25" customHeight="1">
-      <c r="K805" s="37"/>
+      <c r="K805" s="36"/>
     </row>
     <row r="806" ht="14.25" customHeight="1">
-      <c r="K806" s="37"/>
+      <c r="K806" s="36"/>
     </row>
     <row r="807" ht="14.25" customHeight="1">
-      <c r="K807" s="37"/>
+      <c r="K807" s="36"/>
     </row>
     <row r="808" ht="14.25" customHeight="1">
-      <c r="K808" s="37"/>
+      <c r="K808" s="36"/>
     </row>
     <row r="809" ht="14.25" customHeight="1">
-      <c r="K809" s="37"/>
+      <c r="K809" s="36"/>
     </row>
     <row r="810" ht="14.25" customHeight="1">
-      <c r="K810" s="37"/>
+      <c r="K810" s="36"/>
     </row>
     <row r="811" ht="14.25" customHeight="1">
-      <c r="K811" s="37"/>
+      <c r="K811" s="36"/>
     </row>
     <row r="812" ht="14.25" customHeight="1">
-      <c r="K812" s="37"/>
+      <c r="K812" s="36"/>
     </row>
     <row r="813" ht="14.25" customHeight="1">
-      <c r="K813" s="37"/>
+      <c r="K813" s="36"/>
     </row>
     <row r="814" ht="14.25" customHeight="1">
-      <c r="K814" s="37"/>
+      <c r="K814" s="36"/>
     </row>
     <row r="815" ht="14.25" customHeight="1">
-      <c r="K815" s="37"/>
+      <c r="K815" s="36"/>
     </row>
     <row r="816" ht="14.25" customHeight="1">
-      <c r="K816" s="37"/>
+      <c r="K816" s="36"/>
     </row>
     <row r="817" ht="14.25" customHeight="1">
-      <c r="K817" s="37"/>
+      <c r="K817" s="36"/>
     </row>
     <row r="818" ht="14.25" customHeight="1">
-      <c r="K818" s="37"/>
+      <c r="K818" s="36"/>
     </row>
     <row r="819" ht="14.25" customHeight="1">
-      <c r="K819" s="37"/>
+      <c r="K819" s="36"/>
     </row>
     <row r="820" ht="14.25" customHeight="1">
-      <c r="K820" s="37"/>
+      <c r="K820" s="36"/>
     </row>
     <row r="821" ht="14.25" customHeight="1">
-      <c r="K821" s="37"/>
+      <c r="K821" s="36"/>
     </row>
     <row r="822" ht="14.25" customHeight="1">
-      <c r="K822" s="37"/>
+      <c r="K822" s="36"/>
     </row>
     <row r="823" ht="14.25" customHeight="1">
-      <c r="K823" s="37"/>
+      <c r="K823" s="36"/>
     </row>
     <row r="824" ht="14.25" customHeight="1">
-      <c r="K824" s="37"/>
+      <c r="K824" s="36"/>
     </row>
     <row r="825" ht="14.25" customHeight="1">
-      <c r="K825" s="37"/>
+      <c r="K825" s="36"/>
     </row>
     <row r="826" ht="14.25" customHeight="1">
-      <c r="K826" s="37"/>
+      <c r="K826" s="36"/>
     </row>
     <row r="827" ht="14.25" customHeight="1">
-      <c r="K827" s="37"/>
+      <c r="K827" s="36"/>
     </row>
     <row r="828" ht="14.25" customHeight="1">
-      <c r="K828" s="37"/>
+      <c r="K828" s="36"/>
     </row>
     <row r="829" ht="14.25" customHeight="1">
-      <c r="K829" s="37"/>
+      <c r="K829" s="36"/>
     </row>
     <row r="830" ht="14.25" customHeight="1">
-      <c r="K830" s="37"/>
+      <c r="K830" s="36"/>
     </row>
     <row r="831" ht="14.25" customHeight="1">
-      <c r="K831" s="37"/>
+      <c r="K831" s="36"/>
     </row>
     <row r="832" ht="14.25" customHeight="1">
-      <c r="K832" s="37"/>
+      <c r="K832" s="36"/>
     </row>
     <row r="833" ht="14.25" customHeight="1">
-      <c r="K833" s="37"/>
+      <c r="K833" s="36"/>
     </row>
     <row r="834" ht="14.25" customHeight="1">
-      <c r="K834" s="37"/>
+      <c r="K834" s="36"/>
     </row>
     <row r="835" ht="14.25" customHeight="1">
-      <c r="K835" s="37"/>
+      <c r="K835" s="36"/>
     </row>
     <row r="836" ht="14.25" customHeight="1">
-      <c r="K836" s="37"/>
+      <c r="K836" s="36"/>
     </row>
     <row r="837" ht="14.25" customHeight="1">
-      <c r="K837" s="37"/>
+      <c r="K837" s="36"/>
     </row>
     <row r="838" ht="14.25" customHeight="1">
-      <c r="K838" s="37"/>
+      <c r="K838" s="36"/>
     </row>
     <row r="839" ht="14.25" customHeight="1">
-      <c r="K839" s="37"/>
+      <c r="K839" s="36"/>
     </row>
     <row r="840" ht="14.25" customHeight="1">
-      <c r="K840" s="37"/>
+      <c r="K840" s="36"/>
     </row>
     <row r="841" ht="14.25" customHeight="1">
-      <c r="K841" s="37"/>
+      <c r="K841" s="36"/>
     </row>
     <row r="842" ht="14.25" customHeight="1">
-      <c r="K842" s="37"/>
+      <c r="K842" s="36"/>
     </row>
     <row r="843" ht="14.25" customHeight="1">
-      <c r="K843" s="37"/>
+      <c r="K843" s="36"/>
     </row>
     <row r="844" ht="14.25" customHeight="1">
-      <c r="K844" s="37"/>
+      <c r="K844" s="36"/>
     </row>
     <row r="845" ht="14.25" customHeight="1">
-      <c r="K845" s="37"/>
+      <c r="K845" s="36"/>
     </row>
     <row r="846" ht="14.25" customHeight="1">
-      <c r="K846" s="37"/>
+      <c r="K846" s="36"/>
     </row>
     <row r="847" ht="14.25" customHeight="1">
-      <c r="K847" s="37"/>
+      <c r="K847" s="36"/>
     </row>
     <row r="848" ht="14.25" customHeight="1">
-      <c r="K848" s="37"/>
+      <c r="K848" s="36"/>
     </row>
     <row r="849" ht="14.25" customHeight="1">
-      <c r="K849" s="37"/>
+      <c r="K849" s="36"/>
     </row>
     <row r="850" ht="14.25" customHeight="1">
-      <c r="K850" s="37"/>
+      <c r="K850" s="36"/>
     </row>
     <row r="851" ht="14.25" customHeight="1">
-      <c r="K851" s="37"/>
+      <c r="K851" s="36"/>
     </row>
     <row r="852" ht="14.25" customHeight="1">
-      <c r="K852" s="37"/>
+      <c r="K852" s="36"/>
     </row>
     <row r="853" ht="14.25" customHeight="1">
-      <c r="K853" s="37"/>
+      <c r="K853" s="36"/>
     </row>
     <row r="854" ht="14.25" customHeight="1">
-      <c r="K854" s="37"/>
+      <c r="K854" s="36"/>
     </row>
     <row r="855" ht="14.25" customHeight="1">
-      <c r="K855" s="37"/>
+      <c r="K855" s="36"/>
     </row>
     <row r="856" ht="14.25" customHeight="1">
-      <c r="K856" s="37"/>
+      <c r="K856" s="36"/>
     </row>
     <row r="857" ht="14.25" customHeight="1">
-      <c r="K857" s="37"/>
+      <c r="K857" s="36"/>
     </row>
     <row r="858" ht="14.25" customHeight="1">
-      <c r="K858" s="37"/>
+      <c r="K858" s="36"/>
     </row>
     <row r="859" ht="14.25" customHeight="1">
-      <c r="K859" s="37"/>
+      <c r="K859" s="36"/>
     </row>
     <row r="860" ht="14.25" customHeight="1">
-      <c r="K860" s="37"/>
+      <c r="K860" s="36"/>
     </row>
     <row r="861" ht="14.25" customHeight="1">
-      <c r="K861" s="37"/>
+      <c r="K861" s="36"/>
     </row>
     <row r="862" ht="14.25" customHeight="1">
-      <c r="K862" s="37"/>
+      <c r="K862" s="36"/>
     </row>
     <row r="863" ht="14.25" customHeight="1">
-      <c r="K863" s="37"/>
+      <c r="K863" s="36"/>
     </row>
     <row r="864" ht="14.25" customHeight="1">
-      <c r="K864" s="37"/>
+      <c r="K864" s="36"/>
     </row>
     <row r="865" ht="14.25" customHeight="1">
-      <c r="K865" s="37"/>
+      <c r="K865" s="36"/>
     </row>
     <row r="866" ht="14.25" customHeight="1">
-      <c r="K866" s="37"/>
+      <c r="K866" s="36"/>
     </row>
     <row r="867" ht="14.25" customHeight="1">
-      <c r="K867" s="37"/>
+      <c r="K867" s="36"/>
     </row>
     <row r="868" ht="14.25" customHeight="1">
-      <c r="K868" s="37"/>
+      <c r="K868" s="36"/>
     </row>
     <row r="869" ht="14.25" customHeight="1">
-      <c r="K869" s="37"/>
+      <c r="K869" s="36"/>
     </row>
     <row r="870" ht="14.25" customHeight="1">
-      <c r="K870" s="37"/>
+      <c r="K870" s="36"/>
     </row>
     <row r="871" ht="14.25" customHeight="1">
-      <c r="K871" s="37"/>
+      <c r="K871" s="36"/>
     </row>
     <row r="872" ht="14.25" customHeight="1">
-      <c r="K872" s="37"/>
+      <c r="K872" s="36"/>
     </row>
     <row r="873" ht="14.25" customHeight="1">
-      <c r="K873" s="37"/>
+      <c r="K873" s="36"/>
     </row>
     <row r="874" ht="14.25" customHeight="1">
-      <c r="K874" s="37"/>
+      <c r="K874" s="36"/>
     </row>
     <row r="875" ht="14.25" customHeight="1">
-      <c r="K875" s="37"/>
+      <c r="K875" s="36"/>
     </row>
     <row r="876" ht="14.25" customHeight="1">
-      <c r="K876" s="37"/>
+      <c r="K876" s="36"/>
     </row>
     <row r="877" ht="14.25" customHeight="1">
-      <c r="K877" s="37"/>
+      <c r="K877" s="36"/>
     </row>
     <row r="878" ht="14.25" customHeight="1">
-      <c r="K878" s="37"/>
+      <c r="K878" s="36"/>
     </row>
     <row r="879" ht="14.25" customHeight="1">
-      <c r="K879" s="37"/>
+      <c r="K879" s="36"/>
     </row>
     <row r="880" ht="14.25" customHeight="1">
-      <c r="K880" s="37"/>
+      <c r="K880" s="36"/>
     </row>
     <row r="881" ht="14.25" customHeight="1">
-      <c r="K881" s="37"/>
+      <c r="K881" s="36"/>
     </row>
     <row r="882" ht="14.25" customHeight="1">
-      <c r="K882" s="37"/>
+      <c r="K882" s="36"/>
     </row>
     <row r="883" ht="14.25" customHeight="1">
-      <c r="K883" s="37"/>
+      <c r="K883" s="36"/>
     </row>
     <row r="884" ht="14.25" customHeight="1">
-      <c r="K884" s="37"/>
+      <c r="K884" s="36"/>
     </row>
     <row r="885" ht="14.25" customHeight="1">
-      <c r="K885" s="37"/>
+      <c r="K885" s="36"/>
     </row>
     <row r="886" ht="14.25" customHeight="1">
-      <c r="K886" s="37"/>
+      <c r="K886" s="36"/>
     </row>
     <row r="887" ht="14.25" customHeight="1">
-      <c r="K887" s="37"/>
+      <c r="K887" s="36"/>
     </row>
     <row r="888" ht="14.25" customHeight="1">
-      <c r="K888" s="37"/>
+      <c r="K888" s="36"/>
     </row>
     <row r="889" ht="14.25" customHeight="1">
-      <c r="K889" s="37"/>
+      <c r="K889" s="36"/>
     </row>
     <row r="890" ht="14.25" customHeight="1">
-      <c r="K890" s="37"/>
+      <c r="K890" s="36"/>
     </row>
     <row r="891" ht="14.25" customHeight="1">
-      <c r="K891" s="37"/>
+      <c r="K891" s="36"/>
     </row>
     <row r="892" ht="14.25" customHeight="1">
-      <c r="K892" s="37"/>
+      <c r="K892" s="36"/>
     </row>
     <row r="893" ht="14.25" customHeight="1">
-      <c r="K893" s="37"/>
+      <c r="K893" s="36"/>
     </row>
     <row r="894" ht="14.25" customHeight="1">
-      <c r="K894" s="37"/>
+      <c r="K894" s="36"/>
     </row>
     <row r="895" ht="14.25" customHeight="1">
-      <c r="K895" s="37"/>
+      <c r="K895" s="36"/>
     </row>
     <row r="896" ht="14.25" customHeight="1">
-      <c r="K896" s="37"/>
+      <c r="K896" s="36"/>
     </row>
     <row r="897" ht="14.25" customHeight="1">
-      <c r="K897" s="37"/>
+      <c r="K897" s="36"/>
     </row>
     <row r="898" ht="14.25" customHeight="1">
-      <c r="K898" s="37"/>
+      <c r="K898" s="36"/>
     </row>
     <row r="899" ht="14.25" customHeight="1">
-      <c r="K899" s="37"/>
+      <c r="K899" s="36"/>
     </row>
     <row r="900" ht="14.25" customHeight="1">
-      <c r="K900" s="37"/>
+      <c r="K900" s="36"/>
     </row>
     <row r="901" ht="14.25" customHeight="1">
-      <c r="K901" s="37"/>
+      <c r="K901" s="36"/>
     </row>
     <row r="902" ht="14.25" customHeight="1">
-      <c r="K902" s="37"/>
+      <c r="K902" s="36"/>
     </row>
     <row r="903" ht="14.25" customHeight="1">
-      <c r="K903" s="37"/>
+      <c r="K903" s="36"/>
     </row>
     <row r="904" ht="14.25" customHeight="1">
-      <c r="K904" s="37"/>
+      <c r="K904" s="36"/>
     </row>
     <row r="905" ht="14.25" customHeight="1">
-      <c r="K905" s="37"/>
+      <c r="K905" s="36"/>
     </row>
     <row r="906" ht="14.25" customHeight="1">
-      <c r="K906" s="37"/>
+      <c r="K906" s="36"/>
     </row>
     <row r="907" ht="14.25" customHeight="1">
-      <c r="K907" s="37"/>
+      <c r="K907" s="36"/>
     </row>
     <row r="908" ht="14.25" customHeight="1">
-      <c r="K908" s="37"/>
+      <c r="K908" s="36"/>
     </row>
     <row r="909" ht="14.25" customHeight="1">
-      <c r="K909" s="37"/>
+      <c r="K909" s="36"/>
     </row>
     <row r="910" ht="14.25" customHeight="1">
-      <c r="K910" s="37"/>
+      <c r="K910" s="36"/>
     </row>
     <row r="911" ht="14.25" customHeight="1">
-      <c r="K911" s="37"/>
+      <c r="K911" s="36"/>
     </row>
     <row r="912" ht="14.25" customHeight="1">
-      <c r="K912" s="37"/>
+      <c r="K912" s="36"/>
     </row>
     <row r="913" ht="14.25" customHeight="1">
-      <c r="K913" s="37"/>
+      <c r="K913" s="36"/>
     </row>
     <row r="914" ht="14.25" customHeight="1">
-      <c r="K914" s="37"/>
+      <c r="K914" s="36"/>
     </row>
     <row r="915" ht="14.25" customHeight="1">
-      <c r="K915" s="37"/>
+      <c r="K915" s="36"/>
     </row>
     <row r="916" ht="14.25" customHeight="1">
-      <c r="K916" s="37"/>
+      <c r="K916" s="36"/>
     </row>
     <row r="917" ht="14.25" customHeight="1">
-      <c r="K917" s="37"/>
+      <c r="K917" s="36"/>
     </row>
     <row r="918" ht="14.25" customHeight="1">
-      <c r="K918" s="37"/>
+      <c r="K918" s="36"/>
     </row>
     <row r="919" ht="14.25" customHeight="1">
-      <c r="K919" s="37"/>
+      <c r="K919" s="36"/>
     </row>
     <row r="920" ht="14.25" customHeight="1">
-      <c r="K920" s="37"/>
+      <c r="K920" s="36"/>
     </row>
     <row r="921" ht="14.25" customHeight="1">
-      <c r="K921" s="37"/>
+      <c r="K921" s="36"/>
     </row>
     <row r="922" ht="14.25" customHeight="1">
-      <c r="K922" s="37"/>
+      <c r="K922" s="36"/>
     </row>
     <row r="923" ht="14.25" customHeight="1">
-      <c r="K923" s="37"/>
+      <c r="K923" s="36"/>
     </row>
     <row r="924" ht="14.25" customHeight="1">
-      <c r="K924" s="37"/>
+      <c r="K924" s="36"/>
     </row>
     <row r="925" ht="14.25" customHeight="1">
-      <c r="K925" s="37"/>
+      <c r="K925" s="36"/>
     </row>
     <row r="926" ht="14.25" customHeight="1">
-      <c r="K926" s="37"/>
+      <c r="K926" s="36"/>
     </row>
     <row r="927" ht="14.25" customHeight="1">
-      <c r="K927" s="37"/>
+      <c r="K927" s="36"/>
     </row>
     <row r="928" ht="14.25" customHeight="1">
-      <c r="K928" s="37"/>
+      <c r="K928" s="36"/>
     </row>
     <row r="929" ht="14.25" customHeight="1">
-      <c r="K929" s="37"/>
+      <c r="K929" s="36"/>
     </row>
     <row r="930" ht="14.25" customHeight="1">
-      <c r="K930" s="37"/>
+      <c r="K930" s="36"/>
     </row>
     <row r="931" ht="14.25" customHeight="1">
-      <c r="K931" s="37"/>
+      <c r="K931" s="36"/>
     </row>
     <row r="932" ht="14.25" customHeight="1">
-      <c r="K932" s="37"/>
+      <c r="K932" s="36"/>
     </row>
     <row r="933" ht="14.25" customHeight="1">
-      <c r="K933" s="37"/>
+      <c r="K933" s="36"/>
     </row>
     <row r="934" ht="14.25" customHeight="1">
-      <c r="K934" s="37"/>
+      <c r="K934" s="36"/>
     </row>
     <row r="935" ht="14.25" customHeight="1">
-      <c r="K935" s="37"/>
+      <c r="K935" s="36"/>
     </row>
     <row r="936" ht="14.25" customHeight="1">
-      <c r="K936" s="37"/>
+      <c r="K936" s="36"/>
     </row>
     <row r="937" ht="14.25" customHeight="1">
-      <c r="K937" s="37"/>
+      <c r="K937" s="36"/>
     </row>
     <row r="938" ht="14.25" customHeight="1">
-      <c r="K938" s="37"/>
+      <c r="K938" s="36"/>
     </row>
     <row r="939" ht="14.25" customHeight="1">
-      <c r="K939" s="37"/>
+      <c r="K939" s="36"/>
     </row>
     <row r="940" ht="14.25" customHeight="1">
-      <c r="K940" s="37"/>
+      <c r="K940" s="36"/>
     </row>
     <row r="941" ht="14.25" customHeight="1">
-      <c r="K941" s="37"/>
+      <c r="K941" s="36"/>
     </row>
     <row r="942" ht="14.25" customHeight="1">
-      <c r="K942" s="37"/>
+      <c r="K942" s="36"/>
     </row>
     <row r="943" ht="14.25" customHeight="1">
-      <c r="K943" s="37"/>
+      <c r="K943" s="36"/>
     </row>
     <row r="944" ht="14.25" customHeight="1">
-      <c r="K944" s="37"/>
+      <c r="K944" s="36"/>
     </row>
     <row r="945" ht="14.25" customHeight="1">
-      <c r="K945" s="37"/>
+      <c r="K945" s="36"/>
     </row>
     <row r="946" ht="14.25" customHeight="1">
-      <c r="K946" s="37"/>
+      <c r="K946" s="36"/>
     </row>
     <row r="947" ht="14.25" customHeight="1">
-      <c r="K947" s="37"/>
+      <c r="K947" s="36"/>
     </row>
     <row r="948" ht="14.25" customHeight="1">
-      <c r="K948" s="37"/>
+      <c r="K948" s="36"/>
     </row>
     <row r="949" ht="14.25" customHeight="1">
-      <c r="K949" s="37"/>
+      <c r="K949" s="36"/>
     </row>
     <row r="950" ht="14.25" customHeight="1">
-      <c r="K950" s="37"/>
+      <c r="K950" s="36"/>
     </row>
     <row r="951" ht="14.25" customHeight="1">
-      <c r="K951" s="37"/>
+      <c r="K951" s="36"/>
     </row>
     <row r="952" ht="14.25" customHeight="1">
-      <c r="K952" s="37"/>
+      <c r="K952" s="36"/>
     </row>
     <row r="953" ht="14.25" customHeight="1">
-      <c r="K953" s="37"/>
+      <c r="K953" s="36"/>
     </row>
     <row r="954" ht="14.25" customHeight="1">
-      <c r="K954" s="37"/>
+      <c r="K954" s="36"/>
     </row>
     <row r="955" ht="14.25" customHeight="1">
-      <c r="K955" s="37"/>
+      <c r="K955" s="36"/>
     </row>
     <row r="956" ht="14.25" customHeight="1">
-      <c r="K956" s="37"/>
+      <c r="K956" s="36"/>
     </row>
     <row r="957" ht="14.25" customHeight="1">
-      <c r="K957" s="37"/>
+      <c r="K957" s="36"/>
     </row>
     <row r="958" ht="14.25" customHeight="1">
-      <c r="K958" s="37"/>
+      <c r="K958" s="36"/>
     </row>
     <row r="959" ht="14.25" customHeight="1">
-      <c r="K959" s="37"/>
+      <c r="K959" s="36"/>
     </row>
     <row r="960" ht="14.25" customHeight="1">
-      <c r="K960" s="37"/>
+      <c r="K960" s="36"/>
     </row>
     <row r="961" ht="14.25" customHeight="1">
-      <c r="K961" s="37"/>
+      <c r="K961" s="36"/>
     </row>
     <row r="962" ht="14.25" customHeight="1">
-      <c r="K962" s="37"/>
+      <c r="K962" s="36"/>
     </row>
     <row r="963" ht="14.25" customHeight="1">
-      <c r="K963" s="37"/>
+      <c r="K963" s="36"/>
     </row>
     <row r="964" ht="14.25" customHeight="1">
-      <c r="K964" s="37"/>
+      <c r="K964" s="36"/>
     </row>
     <row r="965" ht="14.25" customHeight="1">
-      <c r="K965" s="37"/>
+      <c r="K965" s="36"/>
     </row>
     <row r="966" ht="14.25" customHeight="1">
-      <c r="K966" s="37"/>
+      <c r="K966" s="36"/>
     </row>
     <row r="967" ht="14.25" customHeight="1">
-      <c r="K967" s="37"/>
+      <c r="K967" s="36"/>
     </row>
     <row r="968" ht="14.25" customHeight="1">
-      <c r="K968" s="37"/>
+      <c r="K968" s="36"/>
     </row>
     <row r="969" ht="14.25" customHeight="1">
-      <c r="K969" s="37"/>
+      <c r="K969" s="36"/>
     </row>
     <row r="970" ht="14.25" customHeight="1">
-      <c r="K970" s="37"/>
+      <c r="K970" s="36"/>
     </row>
     <row r="971" ht="14.25" customHeight="1">
-      <c r="K971" s="37"/>
+      <c r="K971" s="36"/>
     </row>
     <row r="972" ht="14.25" customHeight="1">
-      <c r="K972" s="37"/>
+      <c r="K972" s="36"/>
     </row>
     <row r="973" ht="14.25" customHeight="1">
-      <c r="K973" s="37"/>
+      <c r="K973" s="36"/>
     </row>
     <row r="974" ht="14.25" customHeight="1">
-      <c r="K974" s="37"/>
+      <c r="K974" s="36"/>
     </row>
     <row r="975" ht="14.25" customHeight="1">
-      <c r="K975" s="37"/>
+      <c r="K975" s="36"/>
     </row>
     <row r="976" ht="14.25" customHeight="1">
-      <c r="K976" s="37"/>
+      <c r="K976" s="36"/>
     </row>
     <row r="977" ht="14.25" customHeight="1">
-      <c r="K977" s="37"/>
+      <c r="K977" s="36"/>
     </row>
     <row r="978" ht="14.25" customHeight="1">
-      <c r="K978" s="37"/>
+      <c r="K978" s="36"/>
     </row>
     <row r="979" ht="14.25" customHeight="1">
-      <c r="K979" s="37"/>
+      <c r="K979" s="36"/>
     </row>
     <row r="980" ht="14.25" customHeight="1">
-      <c r="K980" s="37"/>
+      <c r="K980" s="36"/>
     </row>
     <row r="981" ht="14.25" customHeight="1">
-      <c r="K981" s="37"/>
+      <c r="K981" s="36"/>
     </row>
     <row r="982" ht="14.25" customHeight="1">
-      <c r="K982" s="37"/>
+      <c r="K982" s="36"/>
     </row>
     <row r="983" ht="14.25" customHeight="1">
-      <c r="K983" s="37"/>
+      <c r="K983" s="36"/>
     </row>
     <row r="984" ht="14.25" customHeight="1">
-      <c r="K984" s="37"/>
+      <c r="K984" s="36"/>
     </row>
     <row r="985" ht="14.25" customHeight="1">
-      <c r="K985" s="37"/>
+      <c r="K985" s="36"/>
     </row>
     <row r="986" ht="14.25" customHeight="1">
-      <c r="K986" s="37"/>
+      <c r="K986" s="36"/>
     </row>
     <row r="987" ht="14.25" customHeight="1">
-      <c r="K987" s="37"/>
+      <c r="K987" s="36"/>
     </row>
     <row r="988" ht="14.25" customHeight="1">
-      <c r="K988" s="37"/>
+      <c r="K988" s="36"/>
     </row>
     <row r="989" ht="14.25" customHeight="1">
-      <c r="K989" s="37"/>
+      <c r="K989" s="36"/>
     </row>
     <row r="990" ht="14.25" customHeight="1">
-      <c r="K990" s="37"/>
+      <c r="K990" s="36"/>
     </row>
     <row r="991" ht="14.25" customHeight="1">
-      <c r="K991" s="37"/>
+      <c r="K991" s="36"/>
     </row>
     <row r="992" ht="14.25" customHeight="1">
-      <c r="K992" s="37"/>
+      <c r="K992" s="36"/>
     </row>
     <row r="993" ht="14.25" customHeight="1">
-      <c r="K993" s="37"/>
+      <c r="K993" s="36"/>
     </row>
     <row r="994" ht="14.25" customHeight="1">
-      <c r="K994" s="37"/>
+      <c r="K994" s="36"/>
     </row>
     <row r="995" ht="14.25" customHeight="1">
-      <c r="K995" s="37"/>
+      <c r="K995" s="36"/>
     </row>
     <row r="996" ht="14.25" customHeight="1">
-      <c r="K996" s="37"/>
+      <c r="K996" s="36"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E20:E24">
+  <conditionalFormatting sqref="E23:E24">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>

</xml_diff>